<commit_message>
Removed ../ in filepaths
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -3951,12 +3951,90 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3999,90 +4077,12 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4161,31 +4161,31 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5072,7 +5072,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5093,86 +5093,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="227" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="239"/>
-      <c r="I1" s="239"/>
-      <c r="J1" s="239"/>
-      <c r="K1" s="240"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="229"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="243" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="218"/>
+      <c r="B3" s="244"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="241" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="242"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="233" t="s">
+      <c r="A5" s="257" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="234"/>
+      <c r="B5" s="258"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="243" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="219"/>
-      <c r="C7" s="219"/>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="218"/>
+      <c r="B7" s="245"/>
+      <c r="C7" s="245"/>
+      <c r="D7" s="245"/>
+      <c r="E7" s="245"/>
+      <c r="F7" s="245"/>
+      <c r="G7" s="245"/>
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="244"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="241" t="s">
+      <c r="A8" s="230" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="242"/>
-      <c r="C8" s="242"/>
-      <c r="D8" s="242"/>
-      <c r="E8" s="242"/>
-      <c r="F8" s="242"/>
-      <c r="G8" s="242"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
-      <c r="K8" s="243"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="231"/>
+      <c r="G8" s="231"/>
+      <c r="H8" s="231"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="231"/>
+      <c r="K8" s="232"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
-      <c r="B9" s="245"/>
-      <c r="C9" s="245"/>
-      <c r="D9" s="245"/>
-      <c r="E9" s="245"/>
-      <c r="F9" s="245"/>
-      <c r="G9" s="245"/>
-      <c r="H9" s="245"/>
-      <c r="I9" s="245"/>
-      <c r="J9" s="245"/>
-      <c r="K9" s="246"/>
+      <c r="A9" s="233"/>
+      <c r="B9" s="234"/>
+      <c r="C9" s="234"/>
+      <c r="D9" s="234"/>
+      <c r="E9" s="234"/>
+      <c r="F9" s="234"/>
+      <c r="G9" s="234"/>
+      <c r="H9" s="234"/>
+      <c r="I9" s="234"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="235"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="157"/>
@@ -5183,62 +5183,62 @@
       <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="220" t="s">
+      <c r="A11" s="246" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="221"/>
-      <c r="C11" s="221"/>
-      <c r="D11" s="222"/>
+      <c r="B11" s="247"/>
+      <c r="C11" s="247"/>
+      <c r="D11" s="248"/>
       <c r="E11" s="88"/>
       <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="223" t="s">
+      <c r="A12" s="249" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="224"/>
-      <c r="C12" s="225" t="s">
+      <c r="B12" s="250"/>
+      <c r="C12" s="251" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="226"/>
+      <c r="D12" s="252"/>
       <c r="E12" s="88"/>
       <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="227"/>
-      <c r="B13" s="228"/>
-      <c r="C13" s="229"/>
-      <c r="D13" s="230"/>
+      <c r="A13" s="253"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="256"/>
       <c r="E13" s="88"/>
       <c r="F13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="220" t="s">
+      <c r="A15" s="246" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="E15" s="220" t="s">
+      <c r="B15" s="248"/>
+      <c r="E15" s="246" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="221"/>
-      <c r="G15" s="221"/>
-      <c r="H15" s="221"/>
-      <c r="I15" s="222"/>
+      <c r="F15" s="247"/>
+      <c r="G15" s="247"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="248"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="231" t="s">
+      <c r="A16" s="241" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="232"/>
+      <c r="B16" s="242"/>
       <c r="D16" s="89"/>
-      <c r="E16" s="247" t="s">
+      <c r="E16" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="248"/>
-      <c r="G16" s="248"/>
-      <c r="H16" s="248"/>
-      <c r="I16" s="249"/>
+      <c r="F16" s="237"/>
+      <c r="G16" s="237"/>
+      <c r="H16" s="237"/>
+      <c r="I16" s="238"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="158" t="s">
@@ -5248,10 +5248,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="90"/>
-      <c r="E17" s="250" t="s">
+      <c r="E17" s="239" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="251"/>
+      <c r="F17" s="240"/>
       <c r="G17" s="214" t="s">
         <v>159</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="H18" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="235" t="s">
+      <c r="I18" s="215" t="s">
         <v>494</v>
       </c>
       <c r="J18" s="82"/>
@@ -5304,7 +5304,7 @@
       <c r="H19" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="235"/>
+      <c r="I19" s="215"/>
       <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="72"/>
-      <c r="I20" s="236"/>
+      <c r="I20" s="216"/>
       <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5343,24 +5343,24 @@
       <c r="A23" s="162"/>
       <c r="B23" s="93"/>
       <c r="C23" s="92"/>
-      <c r="E23" s="215" t="s">
+      <c r="E23" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="237"/>
-      <c r="G23" s="237"/>
-      <c r="H23" s="237"/>
-      <c r="I23" s="216"/>
+      <c r="F23" s="218"/>
+      <c r="G23" s="218"/>
+      <c r="H23" s="218"/>
+      <c r="I23" s="219"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="215" t="s">
+      <c r="A24" s="217" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="216"/>
+      <c r="B24" s="219"/>
       <c r="C24" s="33"/>
-      <c r="E24" s="255" t="s">
+      <c r="E24" s="223" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="256"/>
+      <c r="F24" s="224"/>
       <c r="G24" s="214" t="s">
         <v>159</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="H25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="252" t="s">
+      <c r="I25" s="220" t="s">
         <v>495</v>
       </c>
     </row>
@@ -5413,7 +5413,7 @@
       <c r="H26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="253"/>
+      <c r="I26" s="221"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160" t="s">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
-      <c r="I27" s="254"/>
+      <c r="I27" s="222"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
@@ -5453,22 +5453,22 @@
       <c r="A30" s="161"/>
       <c r="B30" s="118"/>
       <c r="C30" s="90"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="217" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="237"/>
-      <c r="G30" s="237"/>
-      <c r="H30" s="237"/>
-      <c r="I30" s="216"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="218"/>
+      <c r="H30" s="218"/>
+      <c r="I30" s="219"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="162"/>
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
-      <c r="E31" s="257" t="s">
+      <c r="E31" s="225" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="258"/>
+      <c r="F31" s="226"/>
       <c r="G31" s="212" t="s">
         <v>159</v>
       </c>
@@ -5480,10 +5480,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="215" t="s">
+      <c r="A32" s="217" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="216"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="33"/>
       <c r="E32" s="84">
         <v>1</v>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="75"/>
-      <c r="I32" s="235"/>
+      <c r="I32" s="215"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="158" t="s">
@@ -5513,7 +5513,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="34"/>
-      <c r="I33" s="235"/>
+      <c r="I33" s="215"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="159" t="s">
@@ -5528,7 +5528,7 @@
       <c r="F34" s="94"/>
       <c r="G34" s="34"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="235"/>
+      <c r="I34" s="215"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="160" t="s">
@@ -5541,7 +5541,7 @@
       <c r="F35" s="94"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="235"/>
+      <c r="I35" s="215"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="160" t="s">
@@ -5554,7 +5554,7 @@
       <c r="F36" s="94"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="235"/>
+      <c r="I36" s="215"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="160" t="s">
@@ -5567,7 +5567,7 @@
       <c r="F37" s="141"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
-      <c r="I37" s="236"/>
+      <c r="I37" s="216"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="161" t="s">
@@ -5580,17 +5580,17 @@
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="215" t="s">
+      <c r="E40" s="217" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="237"/>
-      <c r="G40" s="237"/>
-      <c r="H40" s="237"/>
-      <c r="I40" s="216"/>
+      <c r="F40" s="218"/>
+      <c r="G40" s="218"/>
+      <c r="H40" s="218"/>
+      <c r="I40" s="219"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="255"/>
-      <c r="F41" s="256"/>
+      <c r="E41" s="223"/>
+      <c r="F41" s="224"/>
       <c r="G41" s="83" t="s">
         <v>159</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="F42" s="94"/>
       <c r="G42" s="34"/>
       <c r="H42" s="75"/>
-      <c r="I42" s="235"/>
+      <c r="I42" s="215"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="84">
@@ -5617,7 +5617,7 @@
       <c r="F43" s="94"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="235"/>
+      <c r="I43" s="215"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="84">
@@ -5626,7 +5626,7 @@
       <c r="F44" s="94"/>
       <c r="G44" s="34"/>
       <c r="H44" s="75"/>
-      <c r="I44" s="235"/>
+      <c r="I44" s="215"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="84">
@@ -5635,7 +5635,7 @@
       <c r="F45" s="94"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="235"/>
+      <c r="I45" s="215"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="84">
@@ -5644,7 +5644,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="235"/>
+      <c r="I46" s="215"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="85">
@@ -5653,25 +5653,11 @@
       <c r="F47" s="141"/>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-      <c r="I47" s="236"/>
+      <c r="I47" s="216"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5687,6 +5673,20 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8080,23 +8080,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
     </row>
@@ -8104,26 +8104,26 @@
       <c r="A2" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="287" t="s">
+      <c r="B2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
     </row>
@@ -8131,21 +8131,21 @@
       <c r="A3" s="202" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="289" t="s">
+      <c r="B3" s="293" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="202" t="s">
         <v>304</v>
       </c>
@@ -8161,25 +8161,25 @@
       <c r="A4" s="205">
         <v>8</v>
       </c>
-      <c r="B4" s="288" t="s">
+      <c r="B4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288" t="s">
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="167" t="s">
         <v>154</v>
       </c>
@@ -8192,21 +8192,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="192"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285" t="s">
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285" t="s">
+      <c r="H5" s="286"/>
+      <c r="I5" s="286"/>
+      <c r="J5" s="286" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="285"/>
-      <c r="L5" s="285"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
       <c r="M5" s="201"/>
       <c r="N5" s="201" t="s">
         <v>391</v>
@@ -8217,23 +8217,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="192"/>
-      <c r="B6" s="285" t="s">
+      <c r="B6" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285" t="s">
+      <c r="C6" s="286"/>
+      <c r="D6" s="286" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285" t="s">
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="286" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="285"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="286"/>
+      <c r="J6" s="286"/>
+      <c r="K6" s="286"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201" t="s">
         <v>392</v>
@@ -8244,57 +8244,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="192"/>
-      <c r="B7" s="285" t="s">
+      <c r="B7" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285" t="s">
+      <c r="C7" s="286"/>
+      <c r="D7" s="286" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="285"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="286"/>
+      <c r="J7" s="286"/>
+      <c r="K7" s="286"/>
+      <c r="L7" s="286"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="165"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="192"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285" t="s">
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
-      <c r="H8" s="285"/>
-      <c r="I8" s="285"/>
-      <c r="J8" s="285"/>
-      <c r="K8" s="285"/>
-      <c r="L8" s="285"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
+      <c r="G8" s="286"/>
+      <c r="H8" s="286"/>
+      <c r="I8" s="286"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+      <c r="L8" s="286"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="165"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -8894,15 +8894,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8919,12 +8916,15 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9016,68 +9016,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
+      <c r="P1" s="291"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="287" t="s">
+      <c r="A2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="B2" s="292"/>
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
-      <c r="P2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
+      <c r="P2" s="287"/>
       <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="B3" s="293"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="202" t="s">
         <v>303</v>
       </c>
@@ -9093,24 +9093,24 @@
       <c r="Q3" s="206"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="288" t="s">
+      <c r="A4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="B4" s="285"/>
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288"/>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="167" t="s">
         <v>254</v>
       </c>
@@ -9125,12 +9125,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="285"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="294" t="s">
         <v>4</v>
       </c>
@@ -9151,12 +9151,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="285"/>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="286"/>
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="294"/>
       <c r="H6" s="294"/>
       <c r="I6" s="294"/>
@@ -9169,12 +9169,12 @@
       <c r="P6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="285"/>
-      <c r="B7" s="285"/>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
+      <c r="A7" s="286"/>
+      <c r="B7" s="286"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="294"/>
       <c r="H7" s="294"/>
       <c r="I7" s="294"/>
@@ -9187,12 +9187,12 @@
       <c r="P7" s="166"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="285"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="294"/>
       <c r="H8" s="294"/>
       <c r="I8" s="294"/>
@@ -9206,17 +9206,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -9549,16 +9549,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9575,6 +9565,16 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Made yml file clone coverney.excel branch in TASBEFlowAnalytics Tutorial
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -3951,20 +3951,116 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3987,102 +4083,6 @@
     <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4161,10 +4161,19 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4177,15 +4186,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5071,8 +5071,8 @@
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5093,86 +5093,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="227" t="s">
+      <c r="A1" s="238" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="228"/>
-      <c r="C1" s="228"/>
-      <c r="D1" s="228"/>
-      <c r="E1" s="228"/>
-      <c r="F1" s="228"/>
-      <c r="G1" s="228"/>
-      <c r="H1" s="228"/>
-      <c r="I1" s="228"/>
-      <c r="J1" s="228"/>
-      <c r="K1" s="229"/>
+      <c r="B1" s="239"/>
+      <c r="C1" s="239"/>
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="239"/>
+      <c r="G1" s="239"/>
+      <c r="H1" s="239"/>
+      <c r="I1" s="239"/>
+      <c r="J1" s="239"/>
+      <c r="K1" s="240"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="243" t="s">
+      <c r="A3" s="217" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="244"/>
+      <c r="B3" s="218"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="231" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="242"/>
+      <c r="B4" s="232"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="257" t="s">
+      <c r="A5" s="233" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="258"/>
+      <c r="B5" s="234"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="243" t="s">
+      <c r="A7" s="217" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="245"/>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
-      <c r="E7" s="245"/>
-      <c r="F7" s="245"/>
-      <c r="G7" s="245"/>
-      <c r="H7" s="245"/>
-      <c r="I7" s="245"/>
-      <c r="J7" s="245"/>
-      <c r="K7" s="244"/>
+      <c r="B7" s="219"/>
+      <c r="C7" s="219"/>
+      <c r="D7" s="219"/>
+      <c r="E7" s="219"/>
+      <c r="F7" s="219"/>
+      <c r="G7" s="219"/>
+      <c r="H7" s="219"/>
+      <c r="I7" s="219"/>
+      <c r="J7" s="219"/>
+      <c r="K7" s="218"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="230" t="s">
+      <c r="A8" s="241" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="231"/>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="231"/>
-      <c r="F8" s="231"/>
-      <c r="G8" s="231"/>
-      <c r="H8" s="231"/>
-      <c r="I8" s="231"/>
-      <c r="J8" s="231"/>
-      <c r="K8" s="232"/>
+      <c r="B8" s="242"/>
+      <c r="C8" s="242"/>
+      <c r="D8" s="242"/>
+      <c r="E8" s="242"/>
+      <c r="F8" s="242"/>
+      <c r="G8" s="242"/>
+      <c r="H8" s="242"/>
+      <c r="I8" s="242"/>
+      <c r="J8" s="242"/>
+      <c r="K8" s="243"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="233"/>
-      <c r="B9" s="234"/>
-      <c r="C9" s="234"/>
-      <c r="D9" s="234"/>
-      <c r="E9" s="234"/>
-      <c r="F9" s="234"/>
-      <c r="G9" s="234"/>
-      <c r="H9" s="234"/>
-      <c r="I9" s="234"/>
-      <c r="J9" s="234"/>
-      <c r="K9" s="235"/>
+      <c r="A9" s="244"/>
+      <c r="B9" s="245"/>
+      <c r="C9" s="245"/>
+      <c r="D9" s="245"/>
+      <c r="E9" s="245"/>
+      <c r="F9" s="245"/>
+      <c r="G9" s="245"/>
+      <c r="H9" s="245"/>
+      <c r="I9" s="245"/>
+      <c r="J9" s="245"/>
+      <c r="K9" s="246"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="157"/>
@@ -5183,62 +5183,62 @@
       <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="246" t="s">
+      <c r="A11" s="220" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="247"/>
-      <c r="C11" s="247"/>
-      <c r="D11" s="248"/>
+      <c r="B11" s="221"/>
+      <c r="C11" s="221"/>
+      <c r="D11" s="222"/>
       <c r="E11" s="88"/>
       <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="249" t="s">
+      <c r="A12" s="223" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="250"/>
-      <c r="C12" s="251" t="s">
+      <c r="B12" s="224"/>
+      <c r="C12" s="225" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="252"/>
+      <c r="D12" s="226"/>
       <c r="E12" s="88"/>
       <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="253"/>
-      <c r="B13" s="254"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="256"/>
+      <c r="A13" s="227"/>
+      <c r="B13" s="228"/>
+      <c r="C13" s="229"/>
+      <c r="D13" s="230"/>
       <c r="E13" s="88"/>
       <c r="F13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="246" t="s">
+      <c r="A15" s="220" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="248"/>
-      <c r="E15" s="246" t="s">
+      <c r="B15" s="222"/>
+      <c r="E15" s="220" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="247"/>
-      <c r="G15" s="247"/>
-      <c r="H15" s="247"/>
-      <c r="I15" s="248"/>
+      <c r="F15" s="221"/>
+      <c r="G15" s="221"/>
+      <c r="H15" s="221"/>
+      <c r="I15" s="222"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="241" t="s">
+      <c r="A16" s="231" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="242"/>
+      <c r="B16" s="232"/>
       <c r="D16" s="89"/>
-      <c r="E16" s="236" t="s">
+      <c r="E16" s="247" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="237"/>
-      <c r="G16" s="237"/>
-      <c r="H16" s="237"/>
-      <c r="I16" s="238"/>
+      <c r="F16" s="248"/>
+      <c r="G16" s="248"/>
+      <c r="H16" s="248"/>
+      <c r="I16" s="249"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="158" t="s">
@@ -5248,10 +5248,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="90"/>
-      <c r="E17" s="239" t="s">
+      <c r="E17" s="250" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="240"/>
+      <c r="F17" s="251"/>
       <c r="G17" s="214" t="s">
         <v>159</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="H18" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="215" t="s">
+      <c r="I18" s="235" t="s">
         <v>494</v>
       </c>
       <c r="J18" s="82"/>
@@ -5304,7 +5304,7 @@
       <c r="H19" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="215"/>
+      <c r="I19" s="235"/>
       <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="72"/>
-      <c r="I20" s="216"/>
+      <c r="I20" s="236"/>
       <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5343,24 +5343,24 @@
       <c r="A23" s="162"/>
       <c r="B23" s="93"/>
       <c r="C23" s="92"/>
-      <c r="E23" s="217" t="s">
+      <c r="E23" s="215" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="218"/>
-      <c r="G23" s="218"/>
-      <c r="H23" s="218"/>
-      <c r="I23" s="219"/>
+      <c r="F23" s="237"/>
+      <c r="G23" s="237"/>
+      <c r="H23" s="237"/>
+      <c r="I23" s="216"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="217" t="s">
+      <c r="A24" s="215" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="219"/>
+      <c r="B24" s="216"/>
       <c r="C24" s="33"/>
-      <c r="E24" s="223" t="s">
+      <c r="E24" s="255" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="224"/>
+      <c r="F24" s="256"/>
       <c r="G24" s="214" t="s">
         <v>159</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="H25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="220" t="s">
+      <c r="I25" s="252" t="s">
         <v>495</v>
       </c>
     </row>
@@ -5413,7 +5413,7 @@
       <c r="H26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="221"/>
+      <c r="I26" s="253"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160" t="s">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
-      <c r="I27" s="222"/>
+      <c r="I27" s="254"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
@@ -5453,22 +5453,22 @@
       <c r="A30" s="161"/>
       <c r="B30" s="118"/>
       <c r="C30" s="90"/>
-      <c r="E30" s="217" t="s">
+      <c r="E30" s="215" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="218"/>
-      <c r="G30" s="218"/>
-      <c r="H30" s="218"/>
-      <c r="I30" s="219"/>
+      <c r="F30" s="237"/>
+      <c r="G30" s="237"/>
+      <c r="H30" s="237"/>
+      <c r="I30" s="216"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="162"/>
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
-      <c r="E31" s="225" t="s">
+      <c r="E31" s="257" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="226"/>
+      <c r="F31" s="258"/>
       <c r="G31" s="212" t="s">
         <v>159</v>
       </c>
@@ -5480,10 +5480,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="217" t="s">
+      <c r="A32" s="215" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="219"/>
+      <c r="B32" s="216"/>
       <c r="C32" s="33"/>
       <c r="E32" s="84">
         <v>1</v>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="75"/>
-      <c r="I32" s="215"/>
+      <c r="I32" s="235"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="158" t="s">
@@ -5513,7 +5513,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="34"/>
-      <c r="I33" s="215"/>
+      <c r="I33" s="235"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="159" t="s">
@@ -5528,7 +5528,7 @@
       <c r="F34" s="94"/>
       <c r="G34" s="34"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="215"/>
+      <c r="I34" s="235"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="160" t="s">
@@ -5541,7 +5541,7 @@
       <c r="F35" s="94"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="215"/>
+      <c r="I35" s="235"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="160" t="s">
@@ -5554,7 +5554,7 @@
       <c r="F36" s="94"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="215"/>
+      <c r="I36" s="235"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="160" t="s">
@@ -5567,7 +5567,7 @@
       <c r="F37" s="141"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
-      <c r="I37" s="216"/>
+      <c r="I37" s="236"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="161" t="s">
@@ -5580,17 +5580,17 @@
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="217" t="s">
+      <c r="E40" s="215" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="218"/>
-      <c r="G40" s="218"/>
-      <c r="H40" s="218"/>
-      <c r="I40" s="219"/>
+      <c r="F40" s="237"/>
+      <c r="G40" s="237"/>
+      <c r="H40" s="237"/>
+      <c r="I40" s="216"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="223"/>
-      <c r="F41" s="224"/>
+      <c r="E41" s="255"/>
+      <c r="F41" s="256"/>
       <c r="G41" s="83" t="s">
         <v>159</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="F42" s="94"/>
       <c r="G42" s="34"/>
       <c r="H42" s="75"/>
-      <c r="I42" s="215"/>
+      <c r="I42" s="235"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="84">
@@ -5617,7 +5617,7 @@
       <c r="F43" s="94"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="215"/>
+      <c r="I43" s="235"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="84">
@@ -5626,7 +5626,7 @@
       <c r="F44" s="94"/>
       <c r="G44" s="34"/>
       <c r="H44" s="75"/>
-      <c r="I44" s="215"/>
+      <c r="I44" s="235"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="84">
@@ -5635,7 +5635,7 @@
       <c r="F45" s="94"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="215"/>
+      <c r="I45" s="235"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="84">
@@ -5644,7 +5644,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="215"/>
+      <c r="I46" s="235"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="85">
@@ -5653,11 +5653,25 @@
       <c r="F47" s="141"/>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-      <c r="I47" s="216"/>
+      <c r="I47" s="236"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5673,20 +5687,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5701,7 +5701,7 @@
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8080,23 +8080,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="286" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
+      <c r="N1" s="286"/>
+      <c r="O1" s="286"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
     </row>
@@ -8104,26 +8104,26 @@
       <c r="A2" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="292" t="s">
+      <c r="B2" s="287" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="292"/>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292" t="s">
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="287" t="s">
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="290" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
     </row>
@@ -8131,21 +8131,21 @@
       <c r="A3" s="202" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="293" t="s">
+      <c r="B3" s="289" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293" t="s">
+      <c r="C3" s="289"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="289" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="289"/>
+      <c r="J3" s="289"/>
+      <c r="K3" s="289"/>
+      <c r="L3" s="289"/>
       <c r="M3" s="202" t="s">
         <v>304</v>
       </c>
@@ -8161,25 +8161,25 @@
       <c r="A4" s="205">
         <v>8</v>
       </c>
-      <c r="B4" s="285" t="s">
+      <c r="B4" s="288" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285" t="s">
+      <c r="C4" s="288"/>
+      <c r="D4" s="288" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="285"/>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285" t="s">
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285" t="s">
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
+      <c r="J4" s="288" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="285"/>
-      <c r="L4" s="285"/>
+      <c r="K4" s="288"/>
+      <c r="L4" s="288"/>
       <c r="M4" s="167" t="s">
         <v>154</v>
       </c>
@@ -8192,21 +8192,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="192"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286" t="s">
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="286"/>
-      <c r="I5" s="286"/>
-      <c r="J5" s="286" t="s">
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="285" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="286"/>
-      <c r="L5" s="286"/>
+      <c r="K5" s="285"/>
+      <c r="L5" s="285"/>
       <c r="M5" s="201"/>
       <c r="N5" s="201" t="s">
         <v>391</v>
@@ -8217,23 +8217,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="192"/>
-      <c r="B6" s="286" t="s">
+      <c r="B6" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286" t="s">
+      <c r="C6" s="285"/>
+      <c r="D6" s="285" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
-      <c r="G6" s="286" t="s">
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="286"/>
-      <c r="I6" s="286"/>
-      <c r="J6" s="286"/>
-      <c r="K6" s="286"/>
-      <c r="L6" s="286"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="285"/>
+      <c r="K6" s="285"/>
+      <c r="L6" s="285"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201" t="s">
         <v>392</v>
@@ -8244,57 +8244,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="192"/>
-      <c r="B7" s="286" t="s">
+      <c r="B7" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="286"/>
-      <c r="D7" s="286" t="s">
+      <c r="C7" s="285"/>
+      <c r="D7" s="285" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
-      <c r="G7" s="286"/>
-      <c r="H7" s="286"/>
-      <c r="I7" s="286"/>
-      <c r="J7" s="286"/>
-      <c r="K7" s="286"/>
-      <c r="L7" s="286"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
+      <c r="H7" s="285"/>
+      <c r="I7" s="285"/>
+      <c r="J7" s="285"/>
+      <c r="K7" s="285"/>
+      <c r="L7" s="285"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="165"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="192"/>
-      <c r="B8" s="286"/>
-      <c r="C8" s="286"/>
-      <c r="D8" s="286" t="s">
+      <c r="B8" s="285"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="286"/>
-      <c r="F8" s="286"/>
-      <c r="G8" s="286"/>
-      <c r="H8" s="286"/>
-      <c r="I8" s="286"/>
-      <c r="J8" s="286"/>
-      <c r="K8" s="286"/>
-      <c r="L8" s="286"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
+      <c r="H8" s="285"/>
+      <c r="I8" s="285"/>
+      <c r="J8" s="285"/>
+      <c r="K8" s="285"/>
+      <c r="L8" s="285"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="165"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="288" t="s">
+      <c r="A10" s="291" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
-      <c r="D10" s="289"/>
-      <c r="E10" s="289"/>
-      <c r="F10" s="289"/>
-      <c r="G10" s="289"/>
-      <c r="H10" s="289"/>
-      <c r="I10" s="290"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="292"/>
+      <c r="I10" s="293"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -8894,12 +8894,15 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8916,15 +8919,12 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9016,68 +9016,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="291" t="s">
+      <c r="A1" s="286" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="291"/>
-      <c r="F1" s="291"/>
-      <c r="G1" s="291"/>
-      <c r="H1" s="291"/>
-      <c r="I1" s="291"/>
-      <c r="J1" s="291"/>
-      <c r="K1" s="291"/>
-      <c r="L1" s="291"/>
-      <c r="M1" s="291"/>
-      <c r="N1" s="291"/>
-      <c r="O1" s="291"/>
-      <c r="P1" s="291"/>
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="286"/>
+      <c r="F1" s="286"/>
+      <c r="G1" s="286"/>
+      <c r="H1" s="286"/>
+      <c r="I1" s="286"/>
+      <c r="J1" s="286"/>
+      <c r="K1" s="286"/>
+      <c r="L1" s="286"/>
+      <c r="M1" s="286"/>
+      <c r="N1" s="286"/>
+      <c r="O1" s="286"/>
+      <c r="P1" s="286"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="292" t="s">
+      <c r="A2" s="287" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="292"/>
-      <c r="C2" s="292"/>
-      <c r="D2" s="292"/>
-      <c r="E2" s="292"/>
-      <c r="F2" s="292"/>
-      <c r="G2" s="292" t="s">
+      <c r="B2" s="287"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="292"/>
-      <c r="I2" s="292"/>
-      <c r="J2" s="292"/>
-      <c r="K2" s="292"/>
-      <c r="L2" s="292"/>
-      <c r="M2" s="287" t="s">
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
+      <c r="J2" s="287"/>
+      <c r="K2" s="287"/>
+      <c r="L2" s="287"/>
+      <c r="M2" s="290" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="287"/>
-      <c r="O2" s="287"/>
-      <c r="P2" s="287"/>
+      <c r="N2" s="290"/>
+      <c r="O2" s="290"/>
+      <c r="P2" s="290"/>
       <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="293" t="s">
+      <c r="A3" s="289" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="293"/>
-      <c r="C3" s="293"/>
-      <c r="D3" s="293"/>
-      <c r="E3" s="293"/>
-      <c r="F3" s="293"/>
-      <c r="G3" s="293" t="s">
+      <c r="B3" s="289"/>
+      <c r="C3" s="289"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="289" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="293"/>
-      <c r="I3" s="293"/>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
+      <c r="H3" s="289"/>
+      <c r="I3" s="289"/>
+      <c r="J3" s="289"/>
+      <c r="K3" s="289"/>
+      <c r="L3" s="289"/>
       <c r="M3" s="202" t="s">
         <v>303</v>
       </c>
@@ -9093,24 +9093,24 @@
       <c r="Q3" s="206"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="285" t="s">
+      <c r="A4" s="288" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="285"/>
-      <c r="C4" s="285"/>
-      <c r="D4" s="285" t="s">
+      <c r="B4" s="288"/>
+      <c r="C4" s="288"/>
+      <c r="D4" s="288" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="285"/>
-      <c r="F4" s="285"/>
-      <c r="G4" s="285" t="s">
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="285"/>
-      <c r="I4" s="285"/>
-      <c r="J4" s="285"/>
-      <c r="K4" s="285"/>
-      <c r="L4" s="285"/>
+      <c r="H4" s="288"/>
+      <c r="I4" s="288"/>
+      <c r="J4" s="288"/>
+      <c r="K4" s="288"/>
+      <c r="L4" s="288"/>
       <c r="M4" s="167" t="s">
         <v>254</v>
       </c>
@@ -9125,12 +9125,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="286"/>
-      <c r="B5" s="286"/>
-      <c r="C5" s="286"/>
-      <c r="D5" s="286"/>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
+      <c r="A5" s="285"/>
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
       <c r="G5" s="294" t="s">
         <v>4</v>
       </c>
@@ -9151,12 +9151,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="286"/>
-      <c r="B6" s="286"/>
-      <c r="C6" s="286"/>
-      <c r="D6" s="286"/>
-      <c r="E6" s="286"/>
-      <c r="F6" s="286"/>
+      <c r="A6" s="285"/>
+      <c r="B6" s="285"/>
+      <c r="C6" s="285"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
       <c r="G6" s="294"/>
       <c r="H6" s="294"/>
       <c r="I6" s="294"/>
@@ -9169,12 +9169,12 @@
       <c r="P6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="286"/>
-      <c r="B7" s="286"/>
-      <c r="C7" s="286"/>
-      <c r="D7" s="286"/>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
+      <c r="A7" s="285"/>
+      <c r="B7" s="285"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
       <c r="G7" s="294"/>
       <c r="H7" s="294"/>
       <c r="I7" s="294"/>
@@ -9187,12 +9187,12 @@
       <c r="P7" s="166"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="286"/>
-      <c r="B8" s="286"/>
-      <c r="C8" s="286"/>
-      <c r="D8" s="286"/>
-      <c r="E8" s="286"/>
-      <c r="F8" s="286"/>
+      <c r="A8" s="285"/>
+      <c r="B8" s="285"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
       <c r="G8" s="294"/>
       <c r="H8" s="294"/>
       <c r="I8" s="294"/>
@@ -9206,17 +9206,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="288" t="s">
+      <c r="A10" s="291" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="289"/>
-      <c r="C10" s="289"/>
-      <c r="D10" s="289"/>
-      <c r="E10" s="289"/>
-      <c r="F10" s="289"/>
-      <c r="G10" s="289"/>
-      <c r="H10" s="289"/>
-      <c r="I10" s="290"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="292"/>
+      <c r="I10" s="293"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -9549,6 +9549,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9565,16 +9575,6 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Adding back the rest of the tests
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -3951,12 +3951,90 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3999,90 +4077,12 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4161,31 +4161,31 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5071,7 +5071,7 @@
   </sheetPr>
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -5093,86 +5093,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="227" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="239"/>
-      <c r="C1" s="239"/>
-      <c r="D1" s="239"/>
-      <c r="E1" s="239"/>
-      <c r="F1" s="239"/>
-      <c r="G1" s="239"/>
-      <c r="H1" s="239"/>
-      <c r="I1" s="239"/>
-      <c r="J1" s="239"/>
-      <c r="K1" s="240"/>
+      <c r="B1" s="228"/>
+      <c r="C1" s="228"/>
+      <c r="D1" s="228"/>
+      <c r="E1" s="228"/>
+      <c r="F1" s="228"/>
+      <c r="G1" s="228"/>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="229"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="87"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="217" t="s">
+      <c r="A3" s="243" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="218"/>
+      <c r="B3" s="244"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="231" t="s">
+      <c r="A4" s="241" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="232"/>
+      <c r="B4" s="242"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="233" t="s">
+      <c r="A5" s="257" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="234"/>
+      <c r="B5" s="258"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="87"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="217" t="s">
+      <c r="A7" s="243" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="219"/>
-      <c r="C7" s="219"/>
-      <c r="D7" s="219"/>
-      <c r="E7" s="219"/>
-      <c r="F7" s="219"/>
-      <c r="G7" s="219"/>
-      <c r="H7" s="219"/>
-      <c r="I7" s="219"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="218"/>
+      <c r="B7" s="245"/>
+      <c r="C7" s="245"/>
+      <c r="D7" s="245"/>
+      <c r="E7" s="245"/>
+      <c r="F7" s="245"/>
+      <c r="G7" s="245"/>
+      <c r="H7" s="245"/>
+      <c r="I7" s="245"/>
+      <c r="J7" s="245"/>
+      <c r="K7" s="244"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="241" t="s">
+      <c r="A8" s="230" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="242"/>
-      <c r="C8" s="242"/>
-      <c r="D8" s="242"/>
-      <c r="E8" s="242"/>
-      <c r="F8" s="242"/>
-      <c r="G8" s="242"/>
-      <c r="H8" s="242"/>
-      <c r="I8" s="242"/>
-      <c r="J8" s="242"/>
-      <c r="K8" s="243"/>
+      <c r="B8" s="231"/>
+      <c r="C8" s="231"/>
+      <c r="D8" s="231"/>
+      <c r="E8" s="231"/>
+      <c r="F8" s="231"/>
+      <c r="G8" s="231"/>
+      <c r="H8" s="231"/>
+      <c r="I8" s="231"/>
+      <c r="J8" s="231"/>
+      <c r="K8" s="232"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="244"/>
-      <c r="B9" s="245"/>
-      <c r="C9" s="245"/>
-      <c r="D9" s="245"/>
-      <c r="E9" s="245"/>
-      <c r="F9" s="245"/>
-      <c r="G9" s="245"/>
-      <c r="H9" s="245"/>
-      <c r="I9" s="245"/>
-      <c r="J9" s="245"/>
-      <c r="K9" s="246"/>
+      <c r="A9" s="233"/>
+      <c r="B9" s="234"/>
+      <c r="C9" s="234"/>
+      <c r="D9" s="234"/>
+      <c r="E9" s="234"/>
+      <c r="F9" s="234"/>
+      <c r="G9" s="234"/>
+      <c r="H9" s="234"/>
+      <c r="I9" s="234"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="235"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="157"/>
@@ -5183,62 +5183,62 @@
       <c r="F10" s="143"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="220" t="s">
+      <c r="A11" s="246" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="221"/>
-      <c r="C11" s="221"/>
-      <c r="D11" s="222"/>
+      <c r="B11" s="247"/>
+      <c r="C11" s="247"/>
+      <c r="D11" s="248"/>
       <c r="E11" s="88"/>
       <c r="F11" s="143"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="223" t="s">
+      <c r="A12" s="249" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="224"/>
-      <c r="C12" s="225" t="s">
+      <c r="B12" s="250"/>
+      <c r="C12" s="251" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="226"/>
+      <c r="D12" s="252"/>
       <c r="E12" s="88"/>
       <c r="F12" s="143"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="227"/>
-      <c r="B13" s="228"/>
-      <c r="C13" s="229"/>
-      <c r="D13" s="230"/>
+      <c r="A13" s="253"/>
+      <c r="B13" s="254"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="256"/>
       <c r="E13" s="88"/>
       <c r="F13" s="143"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="220" t="s">
+      <c r="A15" s="246" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="222"/>
-      <c r="E15" s="220" t="s">
+      <c r="B15" s="248"/>
+      <c r="E15" s="246" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="221"/>
-      <c r="G15" s="221"/>
-      <c r="H15" s="221"/>
-      <c r="I15" s="222"/>
+      <c r="F15" s="247"/>
+      <c r="G15" s="247"/>
+      <c r="H15" s="247"/>
+      <c r="I15" s="248"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="231" t="s">
+      <c r="A16" s="241" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="232"/>
+      <c r="B16" s="242"/>
       <c r="D16" s="89"/>
-      <c r="E16" s="247" t="s">
+      <c r="E16" s="236" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="248"/>
-      <c r="G16" s="248"/>
-      <c r="H16" s="248"/>
-      <c r="I16" s="249"/>
+      <c r="F16" s="237"/>
+      <c r="G16" s="237"/>
+      <c r="H16" s="237"/>
+      <c r="I16" s="238"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="158" t="s">
@@ -5248,10 +5248,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="90"/>
-      <c r="E17" s="250" t="s">
+      <c r="E17" s="239" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="251"/>
+      <c r="F17" s="240"/>
       <c r="G17" s="214" t="s">
         <v>159</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="H18" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="235" t="s">
+      <c r="I18" s="215" t="s">
         <v>494</v>
       </c>
       <c r="J18" s="82"/>
@@ -5304,7 +5304,7 @@
       <c r="H19" s="75" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="235"/>
+      <c r="I19" s="215"/>
       <c r="J19" s="82"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="G20" s="72"/>
       <c r="H20" s="72"/>
-      <c r="I20" s="236"/>
+      <c r="I20" s="216"/>
       <c r="J20" s="82"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5343,24 +5343,24 @@
       <c r="A23" s="162"/>
       <c r="B23" s="93"/>
       <c r="C23" s="92"/>
-      <c r="E23" s="215" t="s">
+      <c r="E23" s="217" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="237"/>
-      <c r="G23" s="237"/>
-      <c r="H23" s="237"/>
-      <c r="I23" s="216"/>
+      <c r="F23" s="218"/>
+      <c r="G23" s="218"/>
+      <c r="H23" s="218"/>
+      <c r="I23" s="219"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="215" t="s">
+      <c r="A24" s="217" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="216"/>
+      <c r="B24" s="219"/>
       <c r="C24" s="33"/>
-      <c r="E24" s="255" t="s">
+      <c r="E24" s="223" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="256"/>
+      <c r="F24" s="224"/>
       <c r="G24" s="214" t="s">
         <v>159</v>
       </c>
@@ -5389,7 +5389,7 @@
       <c r="H25" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="252" t="s">
+      <c r="I25" s="220" t="s">
         <v>495</v>
       </c>
     </row>
@@ -5413,7 +5413,7 @@
       <c r="H26" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="253"/>
+      <c r="I26" s="221"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="160" t="s">
@@ -5429,7 +5429,7 @@
       </c>
       <c r="G27" s="72"/>
       <c r="H27" s="72"/>
-      <c r="I27" s="254"/>
+      <c r="I27" s="222"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
@@ -5453,22 +5453,22 @@
       <c r="A30" s="161"/>
       <c r="B30" s="118"/>
       <c r="C30" s="90"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="217" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="237"/>
-      <c r="G30" s="237"/>
-      <c r="H30" s="237"/>
-      <c r="I30" s="216"/>
+      <c r="F30" s="218"/>
+      <c r="G30" s="218"/>
+      <c r="H30" s="218"/>
+      <c r="I30" s="219"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="162"/>
       <c r="B31" s="92"/>
       <c r="C31" s="92"/>
-      <c r="E31" s="257" t="s">
+      <c r="E31" s="225" t="s">
         <v>472</v>
       </c>
-      <c r="F31" s="258"/>
+      <c r="F31" s="226"/>
       <c r="G31" s="212" t="s">
         <v>159</v>
       </c>
@@ -5480,10 +5480,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="215" t="s">
+      <c r="A32" s="217" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="216"/>
+      <c r="B32" s="219"/>
       <c r="C32" s="33"/>
       <c r="E32" s="84">
         <v>1</v>
@@ -5493,7 +5493,7 @@
       </c>
       <c r="G32" s="34"/>
       <c r="H32" s="75"/>
-      <c r="I32" s="235"/>
+      <c r="I32" s="215"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="158" t="s">
@@ -5513,7 +5513,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="34"/>
-      <c r="I33" s="235"/>
+      <c r="I33" s="215"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="159" t="s">
@@ -5528,7 +5528,7 @@
       <c r="F34" s="94"/>
       <c r="G34" s="34"/>
       <c r="H34" s="75"/>
-      <c r="I34" s="235"/>
+      <c r="I34" s="215"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="160" t="s">
@@ -5541,7 +5541,7 @@
       <c r="F35" s="94"/>
       <c r="G35" s="34"/>
       <c r="H35" s="34"/>
-      <c r="I35" s="235"/>
+      <c r="I35" s="215"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="160" t="s">
@@ -5554,7 +5554,7 @@
       <c r="F36" s="94"/>
       <c r="G36" s="34"/>
       <c r="H36" s="34"/>
-      <c r="I36" s="235"/>
+      <c r="I36" s="215"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="160" t="s">
@@ -5567,7 +5567,7 @@
       <c r="F37" s="141"/>
       <c r="G37" s="72"/>
       <c r="H37" s="72"/>
-      <c r="I37" s="236"/>
+      <c r="I37" s="216"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="161" t="s">
@@ -5580,17 +5580,17 @@
       <c r="B39" s="122"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="215" t="s">
+      <c r="E40" s="217" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="237"/>
-      <c r="G40" s="237"/>
-      <c r="H40" s="237"/>
-      <c r="I40" s="216"/>
+      <c r="F40" s="218"/>
+      <c r="G40" s="218"/>
+      <c r="H40" s="218"/>
+      <c r="I40" s="219"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="255"/>
-      <c r="F41" s="256"/>
+      <c r="E41" s="223"/>
+      <c r="F41" s="224"/>
       <c r="G41" s="83" t="s">
         <v>159</v>
       </c>
@@ -5608,7 +5608,7 @@
       <c r="F42" s="94"/>
       <c r="G42" s="34"/>
       <c r="H42" s="75"/>
-      <c r="I42" s="235"/>
+      <c r="I42" s="215"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="84">
@@ -5617,7 +5617,7 @@
       <c r="F43" s="94"/>
       <c r="G43" s="34"/>
       <c r="H43" s="34"/>
-      <c r="I43" s="235"/>
+      <c r="I43" s="215"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="84">
@@ -5626,7 +5626,7 @@
       <c r="F44" s="94"/>
       <c r="G44" s="34"/>
       <c r="H44" s="75"/>
-      <c r="I44" s="235"/>
+      <c r="I44" s="215"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="84">
@@ -5635,7 +5635,7 @@
       <c r="F45" s="94"/>
       <c r="G45" s="34"/>
       <c r="H45" s="34"/>
-      <c r="I45" s="235"/>
+      <c r="I45" s="215"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="84">
@@ -5644,7 +5644,7 @@
       <c r="F46" s="94"/>
       <c r="G46" s="34"/>
       <c r="H46" s="34"/>
-      <c r="I46" s="235"/>
+      <c r="I46" s="215"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="85">
@@ -5653,25 +5653,11 @@
       <c r="F47" s="141"/>
       <c r="G47" s="72"/>
       <c r="H47" s="72"/>
-      <c r="I47" s="236"/>
+      <c r="I47" s="216"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5687,6 +5673,20 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5700,8 +5700,8 @@
   </sheetPr>
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8080,23 +8080,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
       <c r="P1" s="32"/>
       <c r="Q1" s="32"/>
     </row>
@@ -8104,26 +8104,26 @@
       <c r="A2" s="203" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="287" t="s">
+      <c r="B2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
       <c r="P2" s="89"/>
       <c r="Q2" s="89"/>
     </row>
@@ -8131,21 +8131,21 @@
       <c r="A3" s="202" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="289" t="s">
+      <c r="B3" s="293" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="202" t="s">
         <v>304</v>
       </c>
@@ -8161,25 +8161,25 @@
       <c r="A4" s="205">
         <v>8</v>
       </c>
-      <c r="B4" s="288" t="s">
+      <c r="B4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288" t="s">
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="167" t="s">
         <v>154</v>
       </c>
@@ -8192,21 +8192,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="192"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285" t="s">
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285" t="s">
+      <c r="H5" s="286"/>
+      <c r="I5" s="286"/>
+      <c r="J5" s="286" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="285"/>
-      <c r="L5" s="285"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
       <c r="M5" s="201"/>
       <c r="N5" s="201" t="s">
         <v>391</v>
@@ -8217,23 +8217,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="192"/>
-      <c r="B6" s="285" t="s">
+      <c r="B6" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285" t="s">
+      <c r="C6" s="286"/>
+      <c r="D6" s="286" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285" t="s">
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="286" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="285"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="286"/>
+      <c r="J6" s="286"/>
+      <c r="K6" s="286"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="201"/>
       <c r="N6" s="201" t="s">
         <v>392</v>
@@ -8244,57 +8244,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="192"/>
-      <c r="B7" s="285" t="s">
+      <c r="B7" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285" t="s">
+      <c r="C7" s="286"/>
+      <c r="D7" s="286" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="285"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="286"/>
+      <c r="J7" s="286"/>
+      <c r="K7" s="286"/>
+      <c r="L7" s="286"/>
       <c r="M7" s="201"/>
       <c r="N7" s="201"/>
       <c r="O7" s="165"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="192"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285" t="s">
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
-      <c r="H8" s="285"/>
-      <c r="I8" s="285"/>
-      <c r="J8" s="285"/>
-      <c r="K8" s="285"/>
-      <c r="L8" s="285"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
+      <c r="G8" s="286"/>
+      <c r="H8" s="286"/>
+      <c r="I8" s="286"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+      <c r="L8" s="286"/>
       <c r="M8" s="201"/>
       <c r="N8" s="201"/>
       <c r="O8" s="165"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -8894,15 +8894,12 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8919,12 +8916,15 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9016,68 +9016,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="291" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="286"/>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
-      <c r="N1" s="286"/>
-      <c r="O1" s="286"/>
-      <c r="P1" s="286"/>
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="291"/>
+      <c r="F1" s="291"/>
+      <c r="G1" s="291"/>
+      <c r="H1" s="291"/>
+      <c r="I1" s="291"/>
+      <c r="J1" s="291"/>
+      <c r="K1" s="291"/>
+      <c r="L1" s="291"/>
+      <c r="M1" s="291"/>
+      <c r="N1" s="291"/>
+      <c r="O1" s="291"/>
+      <c r="P1" s="291"/>
       <c r="Q1" s="32"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="287" t="s">
+      <c r="A2" s="292" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="287"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287" t="s">
+      <c r="B2" s="292"/>
+      <c r="C2" s="292"/>
+      <c r="D2" s="292"/>
+      <c r="E2" s="292"/>
+      <c r="F2" s="292"/>
+      <c r="G2" s="292" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
-      <c r="J2" s="287"/>
-      <c r="K2" s="287"/>
-      <c r="L2" s="287"/>
-      <c r="M2" s="290" t="s">
+      <c r="H2" s="292"/>
+      <c r="I2" s="292"/>
+      <c r="J2" s="292"/>
+      <c r="K2" s="292"/>
+      <c r="L2" s="292"/>
+      <c r="M2" s="287" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="290"/>
-      <c r="O2" s="290"/>
-      <c r="P2" s="290"/>
+      <c r="N2" s="287"/>
+      <c r="O2" s="287"/>
+      <c r="P2" s="287"/>
       <c r="Q2" s="89"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="289" t="s">
+      <c r="A3" s="293" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="289"/>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289" t="s">
+      <c r="B3" s="293"/>
+      <c r="C3" s="293"/>
+      <c r="D3" s="293"/>
+      <c r="E3" s="293"/>
+      <c r="F3" s="293"/>
+      <c r="G3" s="293" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="289"/>
-      <c r="I3" s="289"/>
-      <c r="J3" s="289"/>
-      <c r="K3" s="289"/>
-      <c r="L3" s="289"/>
+      <c r="H3" s="293"/>
+      <c r="I3" s="293"/>
+      <c r="J3" s="293"/>
+      <c r="K3" s="293"/>
+      <c r="L3" s="293"/>
       <c r="M3" s="202" t="s">
         <v>303</v>
       </c>
@@ -9093,24 +9093,24 @@
       <c r="Q3" s="206"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="288" t="s">
+      <c r="A4" s="285" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="288"/>
-      <c r="C4" s="288"/>
-      <c r="D4" s="288" t="s">
+      <c r="B4" s="285"/>
+      <c r="C4" s="285"/>
+      <c r="D4" s="285" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288" t="s">
+      <c r="E4" s="285"/>
+      <c r="F4" s="285"/>
+      <c r="G4" s="285" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="288"/>
-      <c r="I4" s="288"/>
-      <c r="J4" s="288"/>
-      <c r="K4" s="288"/>
-      <c r="L4" s="288"/>
+      <c r="H4" s="285"/>
+      <c r="I4" s="285"/>
+      <c r="J4" s="285"/>
+      <c r="K4" s="285"/>
+      <c r="L4" s="285"/>
       <c r="M4" s="167" t="s">
         <v>254</v>
       </c>
@@ -9125,12 +9125,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="285"/>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="294" t="s">
         <v>4</v>
       </c>
@@ -9151,12 +9151,12 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="285"/>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="286"/>
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="294"/>
       <c r="H6" s="294"/>
       <c r="I6" s="294"/>
@@ -9169,12 +9169,12 @@
       <c r="P6" s="168"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="285"/>
-      <c r="B7" s="285"/>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
+      <c r="A7" s="286"/>
+      <c r="B7" s="286"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="294"/>
       <c r="H7" s="294"/>
       <c r="I7" s="294"/>
@@ -9187,12 +9187,12 @@
       <c r="P7" s="166"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="285"/>
-      <c r="B8" s="285"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="294"/>
       <c r="H8" s="294"/>
       <c r="I8" s="294"/>
@@ -9206,17 +9206,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="288" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="293"/>
+      <c r="B10" s="289"/>
+      <c r="C10" s="289"/>
+      <c r="D10" s="289"/>
+      <c r="E10" s="289"/>
+      <c r="F10" s="289"/>
+      <c r="G10" s="289"/>
+      <c r="H10" s="289"/>
+      <c r="I10" s="290"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="132" t="s">
@@ -9549,16 +9549,6 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9575,6 +9565,16 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed typo in test_errors_excel and created transfercurve_excel test
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="500">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -2100,9 +2100,6 @@
     <t>transfercurve</t>
   </si>
   <si>
-    <t>transfercurve/plots</t>
-  </si>
-  <si>
     <t>Missing Output Filename in "Calibration" sheet. Defaulting to exp name.</t>
   </si>
   <si>
@@ -2456,6 +2453,9 @@
   </si>
   <si>
     <t>if true, output statistics file for batch analysis</t>
+  </si>
+  <si>
+    <t>/tmp/</t>
   </si>
 </sst>
 </file>
@@ -3978,20 +3978,116 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4014,102 +4110,6 @@
     <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4188,12 +4188,21 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4204,15 +4213,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5120,86 +5120,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="228" t="s">
+      <c r="A1" s="239" t="s">
         <v>385</v>
       </c>
-      <c r="B1" s="229"/>
-      <c r="C1" s="229"/>
-      <c r="D1" s="229"/>
-      <c r="E1" s="229"/>
-      <c r="F1" s="229"/>
-      <c r="G1" s="229"/>
-      <c r="H1" s="229"/>
-      <c r="I1" s="229"/>
-      <c r="J1" s="229"/>
-      <c r="K1" s="230"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="241"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="86"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="218" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="245"/>
+      <c r="B3" s="219"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="242" t="s">
+      <c r="A4" s="232" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="243"/>
+      <c r="B4" s="233"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="258" t="s">
+      <c r="A5" s="234" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="259"/>
+      <c r="B5" s="235"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="86"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="244" t="s">
+      <c r="A7" s="218" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="245"/>
+      <c r="B7" s="220"/>
+      <c r="C7" s="220"/>
+      <c r="D7" s="220"/>
+      <c r="E7" s="220"/>
+      <c r="F7" s="220"/>
+      <c r="G7" s="220"/>
+      <c r="H7" s="220"/>
+      <c r="I7" s="220"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="219"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="231" t="s">
+      <c r="A8" s="242" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="232"/>
-      <c r="C8" s="232"/>
-      <c r="D8" s="232"/>
-      <c r="E8" s="232"/>
-      <c r="F8" s="232"/>
-      <c r="G8" s="232"/>
-      <c r="H8" s="232"/>
-      <c r="I8" s="232"/>
-      <c r="J8" s="232"/>
-      <c r="K8" s="233"/>
+      <c r="B8" s="243"/>
+      <c r="C8" s="243"/>
+      <c r="D8" s="243"/>
+      <c r="E8" s="243"/>
+      <c r="F8" s="243"/>
+      <c r="G8" s="243"/>
+      <c r="H8" s="243"/>
+      <c r="I8" s="243"/>
+      <c r="J8" s="243"/>
+      <c r="K8" s="244"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="234"/>
-      <c r="B9" s="235"/>
-      <c r="C9" s="235"/>
-      <c r="D9" s="235"/>
-      <c r="E9" s="235"/>
-      <c r="F9" s="235"/>
-      <c r="G9" s="235"/>
-      <c r="H9" s="235"/>
-      <c r="I9" s="235"/>
-      <c r="J9" s="235"/>
-      <c r="K9" s="236"/>
+      <c r="A9" s="245"/>
+      <c r="B9" s="246"/>
+      <c r="C9" s="246"/>
+      <c r="D9" s="246"/>
+      <c r="E9" s="246"/>
+      <c r="F9" s="246"/>
+      <c r="G9" s="246"/>
+      <c r="H9" s="246"/>
+      <c r="I9" s="246"/>
+      <c r="J9" s="246"/>
+      <c r="K9" s="247"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="156"/>
@@ -5210,62 +5210,62 @@
       <c r="F10" s="142"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="247" t="s">
+      <c r="A11" s="221" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="248"/>
-      <c r="C11" s="248"/>
-      <c r="D11" s="249"/>
+      <c r="B11" s="222"/>
+      <c r="C11" s="222"/>
+      <c r="D11" s="223"/>
       <c r="E11" s="87"/>
       <c r="F11" s="142"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="250" t="s">
+      <c r="A12" s="224" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="251"/>
-      <c r="C12" s="252" t="s">
+      <c r="B12" s="225"/>
+      <c r="C12" s="226" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="253"/>
+      <c r="D12" s="227"/>
       <c r="E12" s="87"/>
       <c r="F12" s="142"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="254"/>
-      <c r="B13" s="255"/>
-      <c r="C13" s="256"/>
-      <c r="D13" s="257"/>
+      <c r="A13" s="228"/>
+      <c r="B13" s="229"/>
+      <c r="C13" s="230"/>
+      <c r="D13" s="231"/>
       <c r="E13" s="87"/>
       <c r="F13" s="142"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="247" t="s">
+      <c r="A15" s="221" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="249"/>
-      <c r="E15" s="247" t="s">
+      <c r="B15" s="223"/>
+      <c r="E15" s="221" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="248"/>
-      <c r="G15" s="248"/>
-      <c r="H15" s="248"/>
-      <c r="I15" s="249"/>
+      <c r="F15" s="222"/>
+      <c r="G15" s="222"/>
+      <c r="H15" s="222"/>
+      <c r="I15" s="223"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="242" t="s">
+      <c r="A16" s="232" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="243"/>
+      <c r="B16" s="233"/>
       <c r="D16" s="88"/>
-      <c r="E16" s="237" t="s">
+      <c r="E16" s="248" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="238"/>
-      <c r="G16" s="238"/>
-      <c r="H16" s="238"/>
-      <c r="I16" s="239"/>
+      <c r="F16" s="249"/>
+      <c r="G16" s="249"/>
+      <c r="H16" s="249"/>
+      <c r="I16" s="250"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="157" t="s">
@@ -5275,10 +5275,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="89"/>
-      <c r="E17" s="240" t="s">
+      <c r="E17" s="251" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="241"/>
+      <c r="F17" s="252"/>
       <c r="G17" s="213" t="s">
         <v>159</v>
       </c>
@@ -5308,8 +5308,8 @@
       <c r="H18" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="216" t="s">
-        <v>494</v>
+      <c r="I18" s="236" t="s">
+        <v>493</v>
       </c>
       <c r="J18" s="81"/>
     </row>
@@ -5331,7 +5331,7 @@
       <c r="H19" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="216"/>
+      <c r="I19" s="236"/>
       <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5348,7 +5348,7 @@
       </c>
       <c r="G20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="217"/>
+      <c r="I20" s="237"/>
       <c r="J20" s="81"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5370,24 +5370,24 @@
       <c r="A23" s="161"/>
       <c r="B23" s="92"/>
       <c r="C23" s="91"/>
-      <c r="E23" s="218" t="s">
+      <c r="E23" s="216" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="219"/>
-      <c r="G23" s="219"/>
-      <c r="H23" s="219"/>
-      <c r="I23" s="220"/>
+      <c r="F23" s="238"/>
+      <c r="G23" s="238"/>
+      <c r="H23" s="238"/>
+      <c r="I23" s="217"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="218" t="s">
+      <c r="A24" s="216" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="220"/>
+      <c r="B24" s="217"/>
       <c r="C24" s="32"/>
-      <c r="E24" s="224" t="s">
+      <c r="E24" s="256" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="225"/>
+      <c r="F24" s="257"/>
       <c r="G24" s="213" t="s">
         <v>159</v>
       </c>
@@ -5416,8 +5416,8 @@
       <c r="H25" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="221" t="s">
-        <v>495</v>
+      <c r="I25" s="253" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
@@ -5440,7 +5440,7 @@
       <c r="H26" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="222"/>
+      <c r="I26" s="254"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="159" t="s">
@@ -5456,7 +5456,7 @@
       </c>
       <c r="G27" s="71"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="223"/>
+      <c r="I27" s="255"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="159" t="s">
@@ -5480,22 +5480,22 @@
       <c r="A30" s="160"/>
       <c r="B30" s="117"/>
       <c r="C30" s="89"/>
-      <c r="E30" s="218" t="s">
+      <c r="E30" s="216" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="219"/>
-      <c r="G30" s="219"/>
-      <c r="H30" s="219"/>
-      <c r="I30" s="220"/>
+      <c r="F30" s="238"/>
+      <c r="G30" s="238"/>
+      <c r="H30" s="238"/>
+      <c r="I30" s="217"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="161"/>
       <c r="B31" s="91"/>
       <c r="C31" s="91"/>
-      <c r="E31" s="226" t="s">
-        <v>472</v>
-      </c>
-      <c r="F31" s="227"/>
+      <c r="E31" s="258" t="s">
+        <v>471</v>
+      </c>
+      <c r="F31" s="259"/>
       <c r="G31" s="211" t="s">
         <v>159</v>
       </c>
@@ -5507,10 +5507,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="218" t="s">
+      <c r="A32" s="216" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="220"/>
+      <c r="B32" s="217"/>
       <c r="C32" s="32"/>
       <c r="E32" s="83">
         <v>1</v>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="74"/>
-      <c r="I32" s="216"/>
+      <c r="I32" s="236"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="157" t="s">
@@ -5540,7 +5540,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="216"/>
+      <c r="I33" s="236"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="158" t="s">
@@ -5555,7 +5555,7 @@
       <c r="F34" s="93"/>
       <c r="G34" s="33"/>
       <c r="H34" s="74"/>
-      <c r="I34" s="216"/>
+      <c r="I34" s="236"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="159" t="s">
@@ -5568,7 +5568,7 @@
       <c r="F35" s="93"/>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
-      <c r="I35" s="216"/>
+      <c r="I35" s="236"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="159" t="s">
@@ -5581,7 +5581,7 @@
       <c r="F36" s="93"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
-      <c r="I36" s="216"/>
+      <c r="I36" s="236"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="159" t="s">
@@ -5594,7 +5594,7 @@
       <c r="F37" s="140"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="217"/>
+      <c r="I37" s="237"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="160" t="s">
@@ -5607,17 +5607,17 @@
       <c r="B39" s="121"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="218" t="s">
+      <c r="E40" s="216" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="219"/>
-      <c r="G40" s="219"/>
-      <c r="H40" s="219"/>
-      <c r="I40" s="220"/>
+      <c r="F40" s="238"/>
+      <c r="G40" s="238"/>
+      <c r="H40" s="238"/>
+      <c r="I40" s="217"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="224"/>
-      <c r="F41" s="225"/>
+      <c r="E41" s="256"/>
+      <c r="F41" s="257"/>
       <c r="G41" s="82" t="s">
         <v>159</v>
       </c>
@@ -5635,7 +5635,7 @@
       <c r="F42" s="93"/>
       <c r="G42" s="33"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="216"/>
+      <c r="I42" s="236"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="83">
@@ -5644,7 +5644,7 @@
       <c r="F43" s="93"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="216"/>
+      <c r="I43" s="236"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="83">
@@ -5653,7 +5653,7 @@
       <c r="F44" s="93"/>
       <c r="G44" s="33"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="216"/>
+      <c r="I44" s="236"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="83">
@@ -5662,7 +5662,7 @@
       <c r="F45" s="93"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
-      <c r="I45" s="216"/>
+      <c r="I45" s="236"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="83">
@@ -5671,7 +5671,7 @@
       <c r="F46" s="93"/>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
-      <c r="I46" s="216"/>
+      <c r="I46" s="236"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="84">
@@ -5680,11 +5680,25 @@
       <c r="F47" s="140"/>
       <c r="G47" s="71"/>
       <c r="H47" s="71"/>
-      <c r="I47" s="217"/>
+      <c r="I47" s="237"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5700,20 +5714,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5727,7 +5727,7 @@
   </sheetPr>
   <dimension ref="A1:Q71"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -5843,7 +5843,7 @@
         <v>8</v>
       </c>
       <c r="J4" s="199" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -5853,7 +5853,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="78" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C5" s="109">
         <v>0.1</v>
@@ -5878,7 +5878,7 @@
       </c>
       <c r="J5" s="112"/>
       <c r="K5" s="212" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5912,7 +5912,7 @@
       </c>
       <c r="J6" s="112"/>
       <c r="K6" s="212" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5942,7 +5942,7 @@
       </c>
       <c r="J7" s="112"/>
       <c r="K7" s="212" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="8" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -5976,7 +5976,7 @@
       </c>
       <c r="J8" s="112"/>
       <c r="K8" s="212" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6008,7 +6008,7 @@
       </c>
       <c r="J9" s="112"/>
       <c r="K9" s="212" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6038,7 +6038,7 @@
       </c>
       <c r="J10" s="112"/>
       <c r="K10" s="212" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6068,7 +6068,7 @@
       </c>
       <c r="J11" s="112"/>
       <c r="K11" s="212" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6098,7 +6098,7 @@
       </c>
       <c r="J12" s="112"/>
       <c r="K12" s="212" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6128,7 +6128,7 @@
       </c>
       <c r="J13" s="112"/>
       <c r="K13" s="212" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6160,7 +6160,7 @@
       </c>
       <c r="J14" s="112"/>
       <c r="K14" s="212" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6194,7 +6194,7 @@
       </c>
       <c r="J15" s="112"/>
       <c r="K15" s="212" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6224,7 +6224,7 @@
       </c>
       <c r="J16" s="112"/>
       <c r="K16" s="212" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6258,7 +6258,7 @@
       </c>
       <c r="J17" s="112"/>
       <c r="K17" s="212" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6292,7 +6292,7 @@
       </c>
       <c r="J18" s="112"/>
       <c r="K18" s="212" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6316,7 +6316,7 @@
         <v>5</v>
       </c>
       <c r="K19" s="212" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6340,7 +6340,7 @@
         <v>5</v>
       </c>
       <c r="K20" s="212" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6364,7 +6364,7 @@
         <v>5</v>
       </c>
       <c r="K21" s="212" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6388,7 +6388,7 @@
         <v>5</v>
       </c>
       <c r="K22" s="212" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6412,7 +6412,7 @@
         <v>5</v>
       </c>
       <c r="K23" s="212" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -6436,7 +6436,7 @@
         <v>5</v>
       </c>
       <c r="K24" s="212" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -6460,7 +6460,7 @@
         <v>5</v>
       </c>
       <c r="K25" s="212" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6505,19 +6505,19 @@
         <v>388</v>
       </c>
       <c r="G28" s="194" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H28" s="198" t="s">
         <v>270</v>
       </c>
       <c r="I28" s="198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="J28" s="198" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="K28" s="198" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="L28" s="123" t="s">
         <v>273</v>
@@ -6559,16 +6559,16 @@
         <v>374</v>
       </c>
       <c r="H29" s="96" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I29" s="96" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="J29" s="96" t="s">
+        <v>447</v>
+      </c>
+      <c r="K29" s="96" t="s">
         <v>448</v>
-      </c>
-      <c r="K29" s="96" t="s">
-        <v>449</v>
       </c>
       <c r="L29" s="96" t="s">
         <v>94</v>
@@ -6592,24 +6592,24 @@
     <row r="30" spans="1:17" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="146"/>
       <c r="B30" s="208" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C30" s="97"/>
       <c r="D30" s="97"/>
       <c r="E30" s="153"/>
       <c r="F30" s="153"/>
       <c r="G30" s="153" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H30" s="153"/>
       <c r="I30" s="153" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="J30" s="153">
         <v>3</v>
       </c>
       <c r="K30" s="153" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="L30" s="153">
         <v>100</v>
@@ -6720,7 +6720,7 @@
         <v>317</v>
       </c>
       <c r="C40" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D40" s="180" t="s">
         <v>375</v>
@@ -6734,7 +6734,7 @@
         <v>342</v>
       </c>
       <c r="C41" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D41" s="193" t="s">
         <v>339</v>
@@ -6748,7 +6748,7 @@
         <v>343</v>
       </c>
       <c r="C42" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D42" s="180" t="s">
         <v>340</v>
@@ -6762,7 +6762,7 @@
         <v>344</v>
       </c>
       <c r="C43" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D43" s="180" t="s">
         <v>362</v>
@@ -6776,7 +6776,7 @@
         <v>345</v>
       </c>
       <c r="C44" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D44" s="183" t="s">
         <v>341</v>
@@ -6784,184 +6784,184 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B45" t="s">
         <v>318</v>
       </c>
       <c r="C45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D45" s="193" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B46" t="s">
         <v>318</v>
       </c>
       <c r="C46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D46" s="193" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B47" t="s">
         <v>318</v>
       </c>
       <c r="C47" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D47" s="193" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B48" t="s">
         <v>318</v>
       </c>
       <c r="C48" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D48" s="193" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B49" t="s">
         <v>318</v>
       </c>
       <c r="C49" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D49" s="193" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B50" t="s">
         <v>346</v>
       </c>
       <c r="C50" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D50" s="193" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>421</v>
+      </c>
+      <c r="B51" t="s">
         <v>422</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
+        <v>451</v>
+      </c>
+      <c r="D51" s="193" t="s">
         <v>423</v>
-      </c>
-      <c r="C51" t="s">
-        <v>452</v>
-      </c>
-      <c r="D51" s="193" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B52" t="s">
         <v>384</v>
       </c>
       <c r="C52" t="s">
+        <v>451</v>
+      </c>
+      <c r="D52" s="180" t="s">
         <v>452</v>
-      </c>
-      <c r="D52" s="180" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>424</v>
+      </c>
+      <c r="B53" t="s">
         <v>425</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
+        <v>451</v>
+      </c>
+      <c r="D53" s="193" t="s">
         <v>426</v>
-      </c>
-      <c r="C53" t="s">
-        <v>452</v>
-      </c>
-      <c r="D53" s="193" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>424</v>
+      </c>
+      <c r="B54" t="s">
         <v>425</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>451</v>
+      </c>
+      <c r="D54" s="193" t="s">
         <v>426</v>
-      </c>
-      <c r="C54" t="s">
-        <v>452</v>
-      </c>
-      <c r="D54" s="193" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>424</v>
+      </c>
+      <c r="B55" t="s">
         <v>425</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>451</v>
+      </c>
+      <c r="D55" s="193" t="s">
         <v>426</v>
-      </c>
-      <c r="C55" t="s">
-        <v>452</v>
-      </c>
-      <c r="D55" s="193" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>424</v>
+      </c>
+      <c r="B56" t="s">
         <v>425</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
+        <v>451</v>
+      </c>
+      <c r="D56" s="193" t="s">
         <v>426</v>
-      </c>
-      <c r="C56" t="s">
-        <v>452</v>
-      </c>
-      <c r="D56" s="193" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>424</v>
+      </c>
+      <c r="B57" t="s">
         <v>425</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
+        <v>451</v>
+      </c>
+      <c r="D57" s="193" t="s">
         <v>426</v>
-      </c>
-      <c r="C57" t="s">
-        <v>452</v>
-      </c>
-      <c r="D57" s="193" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -6972,10 +6972,10 @@
         <v>390</v>
       </c>
       <c r="C58" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D58" s="180" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -6986,10 +6986,10 @@
         <v>390</v>
       </c>
       <c r="C59" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D59" s="180" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -7000,10 +7000,10 @@
         <v>390</v>
       </c>
       <c r="C60" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D60" s="180" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -7014,10 +7014,10 @@
         <v>390</v>
       </c>
       <c r="C61" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D61" s="180" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -7028,10 +7028,10 @@
         <v>390</v>
       </c>
       <c r="C62" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D62" s="180" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -7042,10 +7042,10 @@
         <v>390</v>
       </c>
       <c r="C63" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D63" s="180" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -7056,10 +7056,10 @@
         <v>390</v>
       </c>
       <c r="C64" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D64" s="180" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -7070,10 +7070,10 @@
         <v>390</v>
       </c>
       <c r="C65" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D65" s="180" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -7084,10 +7084,10 @@
         <v>390</v>
       </c>
       <c r="C66" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D66" s="180" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -7098,10 +7098,10 @@
         <v>390</v>
       </c>
       <c r="C67" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D67" s="180" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -7112,10 +7112,10 @@
         <v>390</v>
       </c>
       <c r="C68" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D68" s="180" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -7126,10 +7126,10 @@
         <v>390</v>
       </c>
       <c r="C69" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D69" s="180" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -7140,10 +7140,10 @@
         <v>390</v>
       </c>
       <c r="C70" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D70" s="180" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -7154,10 +7154,10 @@
         <v>390</v>
       </c>
       <c r="C71" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D71" s="180" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
   </sheetData>
@@ -7235,8 +7235,8 @@
   </sheetPr>
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7775,12 +7775,12 @@
     <row r="28" spans="1:10" s="113" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="146"/>
       <c r="B28" s="209" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C28" s="190"/>
       <c r="D28" s="122"/>
       <c r="E28" s="153" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
@@ -7880,7 +7880,7 @@
         <v>317</v>
       </c>
       <c r="C38" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D38" s="180" t="s">
         <v>375</v>
@@ -7894,7 +7894,7 @@
         <v>342</v>
       </c>
       <c r="C39" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D39" s="193" t="s">
         <v>339</v>
@@ -7908,7 +7908,7 @@
         <v>343</v>
       </c>
       <c r="C40" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D40" s="180" t="s">
         <v>340</v>
@@ -7922,7 +7922,7 @@
         <v>344</v>
       </c>
       <c r="C41" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D41" s="180" t="s">
         <v>362</v>
@@ -7936,7 +7936,7 @@
         <v>345</v>
       </c>
       <c r="C42" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D42" s="183" t="s">
         <v>341</v>
@@ -7950,7 +7950,7 @@
         <v>318</v>
       </c>
       <c r="C43" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D43" s="193" t="s">
         <v>377</v>
@@ -7964,7 +7964,7 @@
         <v>379</v>
       </c>
       <c r="C44" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D44" s="193" t="s">
         <v>380</v>
@@ -7978,10 +7978,10 @@
         <v>379</v>
       </c>
       <c r="C45" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D45" s="193" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -7992,7 +7992,7 @@
         <v>379</v>
       </c>
       <c r="C46" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D46" s="193" t="s">
         <v>381</v>
@@ -8006,7 +8006,7 @@
         <v>379</v>
       </c>
       <c r="C47" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D47" s="193" t="s">
         <v>382</v>
@@ -8017,13 +8017,13 @@
         <v>338</v>
       </c>
       <c r="B48" t="s">
+        <v>469</v>
+      </c>
+      <c r="C48" t="s">
+        <v>468</v>
+      </c>
+      <c r="D48" s="183" t="s">
         <v>470</v>
-      </c>
-      <c r="C48" t="s">
-        <v>469</v>
-      </c>
-      <c r="D48" s="183" t="s">
-        <v>471</v>
       </c>
     </row>
   </sheetData>
@@ -8107,23 +8107,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="287" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="O1" s="292"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
     </row>
@@ -8131,26 +8131,26 @@
       <c r="A2" s="202" t="s">
         <v>360</v>
       </c>
-      <c r="B2" s="293" t="s">
+      <c r="B2" s="288" t="s">
         <v>282</v>
       </c>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293" t="s">
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="288" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
@@ -8158,21 +8158,21 @@
       <c r="A3" s="201" t="s">
         <v>361</v>
       </c>
-      <c r="B3" s="294" t="s">
+      <c r="B3" s="290" t="s">
         <v>298</v>
       </c>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294" t="s">
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="201" t="s">
         <v>304</v>
       </c>
@@ -8188,25 +8188,25 @@
       <c r="A4" s="204">
         <v>8</v>
       </c>
-      <c r="B4" s="286" t="s">
+      <c r="B4" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="C4" s="286"/>
-      <c r="D4" s="286" t="s">
+      <c r="C4" s="289"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="286"/>
-      <c r="I4" s="286"/>
-      <c r="J4" s="286" t="s">
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="286"/>
-      <c r="L4" s="286"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="166" t="s">
         <v>154</v>
       </c>
@@ -8219,21 +8219,21 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="191"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
-      <c r="G5" s="287" t="s">
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
+      <c r="G5" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="287"/>
-      <c r="I5" s="287"/>
-      <c r="J5" s="287" t="s">
+      <c r="H5" s="286"/>
+      <c r="I5" s="286"/>
+      <c r="J5" s="286" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="287"/>
-      <c r="L5" s="287"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
       <c r="M5" s="200"/>
       <c r="N5" s="200" t="s">
         <v>391</v>
@@ -8244,23 +8244,23 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="191"/>
-      <c r="B6" s="287" t="s">
+      <c r="B6" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C6" s="287"/>
-      <c r="D6" s="287" t="s">
+      <c r="C6" s="286"/>
+      <c r="D6" s="286" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
-      <c r="G6" s="287" t="s">
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
+      <c r="G6" s="286" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="287"/>
-      <c r="I6" s="287"/>
-      <c r="J6" s="287"/>
-      <c r="K6" s="287"/>
-      <c r="L6" s="287"/>
+      <c r="H6" s="286"/>
+      <c r="I6" s="286"/>
+      <c r="J6" s="286"/>
+      <c r="K6" s="286"/>
+      <c r="L6" s="286"/>
       <c r="M6" s="200"/>
       <c r="N6" s="200" t="s">
         <v>392</v>
@@ -8271,57 +8271,57 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="191"/>
-      <c r="B7" s="287" t="s">
+      <c r="B7" s="286" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="287"/>
-      <c r="D7" s="287" t="s">
+      <c r="C7" s="286"/>
+      <c r="D7" s="286" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="287"/>
-      <c r="F7" s="287"/>
-      <c r="G7" s="287"/>
-      <c r="H7" s="287"/>
-      <c r="I7" s="287"/>
-      <c r="J7" s="287"/>
-      <c r="K7" s="287"/>
-      <c r="L7" s="287"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="286"/>
+      <c r="J7" s="286"/>
+      <c r="K7" s="286"/>
+      <c r="L7" s="286"/>
       <c r="M7" s="200"/>
       <c r="N7" s="200"/>
       <c r="O7" s="164"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="191"/>
-      <c r="B8" s="287"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287" t="s">
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
-      <c r="G8" s="287"/>
-      <c r="H8" s="287"/>
-      <c r="I8" s="287"/>
-      <c r="J8" s="287"/>
-      <c r="K8" s="287"/>
-      <c r="L8" s="287"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
+      <c r="G8" s="286"/>
+      <c r="H8" s="286"/>
+      <c r="I8" s="286"/>
+      <c r="J8" s="286"/>
+      <c r="K8" s="286"/>
+      <c r="L8" s="286"/>
       <c r="M8" s="200"/>
       <c r="N8" s="200"/>
       <c r="O8" s="164"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="292" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="290"/>
-      <c r="C10" s="290"/>
-      <c r="D10" s="290"/>
-      <c r="E10" s="290"/>
-      <c r="F10" s="290"/>
-      <c r="G10" s="290"/>
-      <c r="H10" s="290"/>
-      <c r="I10" s="291"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="131" t="s">
@@ -8493,7 +8493,7 @@
         <v>317</v>
       </c>
       <c r="C23" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D23" s="180" t="s">
         <v>375</v>
@@ -8507,7 +8507,7 @@
         <v>342</v>
       </c>
       <c r="C24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D24" s="193" t="s">
         <v>339</v>
@@ -8521,7 +8521,7 @@
         <v>343</v>
       </c>
       <c r="C25" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D25" s="180" t="s">
         <v>340</v>
@@ -8535,7 +8535,7 @@
         <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D26" s="180" t="s">
         <v>362</v>
@@ -8549,7 +8549,7 @@
         <v>345</v>
       </c>
       <c r="C27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D27" s="183" t="s">
         <v>341</v>
@@ -8563,10 +8563,10 @@
         <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D28" s="193" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -8577,10 +8577,10 @@
         <v>318</v>
       </c>
       <c r="C29" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D29" s="193" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -8591,10 +8591,10 @@
         <v>318</v>
       </c>
       <c r="C30" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D30" s="193" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -8605,7 +8605,7 @@
         <v>318</v>
       </c>
       <c r="C31" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D31" s="193" t="s">
         <v>348</v>
@@ -8619,10 +8619,10 @@
         <v>318</v>
       </c>
       <c r="C32" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D32" s="193" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -8633,10 +8633,10 @@
         <v>346</v>
       </c>
       <c r="C33" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D33" s="193" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -8647,10 +8647,10 @@
         <v>384</v>
       </c>
       <c r="C34" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D34" s="180" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -8661,10 +8661,10 @@
         <v>390</v>
       </c>
       <c r="C35" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D35" s="180" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -8675,10 +8675,10 @@
         <v>390</v>
       </c>
       <c r="C36" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D36" s="180" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -8689,10 +8689,10 @@
         <v>390</v>
       </c>
       <c r="C37" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D37" s="180" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -8703,10 +8703,10 @@
         <v>390</v>
       </c>
       <c r="C38" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D38" s="180" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -8717,10 +8717,10 @@
         <v>390</v>
       </c>
       <c r="C39" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D39" s="180" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -8731,10 +8731,10 @@
         <v>390</v>
       </c>
       <c r="C40" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D40" s="180" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -8745,10 +8745,10 @@
         <v>390</v>
       </c>
       <c r="C41" t="s">
+        <v>454</v>
+      </c>
+      <c r="D41" s="180" t="s">
         <v>455</v>
-      </c>
-      <c r="D41" s="180" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -8759,10 +8759,10 @@
         <v>390</v>
       </c>
       <c r="C42" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D42" s="180" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -8773,10 +8773,10 @@
         <v>390</v>
       </c>
       <c r="C43" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D43" s="180" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -8787,10 +8787,10 @@
         <v>390</v>
       </c>
       <c r="C44" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D44" s="180" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -8801,10 +8801,10 @@
         <v>390</v>
       </c>
       <c r="C45" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D45" s="180" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -8815,10 +8815,10 @@
         <v>390</v>
       </c>
       <c r="C46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D46" s="180" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -8829,10 +8829,10 @@
         <v>390</v>
       </c>
       <c r="C47" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D47" s="180" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -8843,10 +8843,10 @@
         <v>390</v>
       </c>
       <c r="C48" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D48" s="180" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -8857,10 +8857,10 @@
         <v>390</v>
       </c>
       <c r="C49" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D49" s="180" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -8871,10 +8871,10 @@
         <v>390</v>
       </c>
       <c r="C50" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D50" s="180" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -8885,10 +8885,10 @@
         <v>390</v>
       </c>
       <c r="C51" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D51" s="180" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -8899,10 +8899,10 @@
         <v>346</v>
       </c>
       <c r="C52" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D52" s="193" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -8913,20 +8913,23 @@
         <v>384</v>
       </c>
       <c r="C53" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D53" s="180" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="G6:I6"/>
@@ -8943,15 +8946,12 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9017,8 +9017,8 @@
   </sheetPr>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9043,68 +9043,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="292" t="s">
+      <c r="A1" s="287" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="292"/>
-      <c r="C1" s="292"/>
-      <c r="D1" s="292"/>
-      <c r="E1" s="292"/>
-      <c r="F1" s="292"/>
-      <c r="G1" s="292"/>
-      <c r="H1" s="292"/>
-      <c r="I1" s="292"/>
-      <c r="J1" s="292"/>
-      <c r="K1" s="292"/>
-      <c r="L1" s="292"/>
-      <c r="M1" s="292"/>
-      <c r="N1" s="292"/>
-      <c r="O1" s="292"/>
-      <c r="P1" s="292"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="293" t="s">
+      <c r="A2" s="288" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="293"/>
-      <c r="C2" s="293"/>
-      <c r="D2" s="293"/>
-      <c r="E2" s="293"/>
-      <c r="F2" s="293"/>
-      <c r="G2" s="293" t="s">
+      <c r="B2" s="288"/>
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="293"/>
-      <c r="I2" s="293"/>
-      <c r="J2" s="293"/>
-      <c r="K2" s="293"/>
-      <c r="L2" s="293"/>
-      <c r="M2" s="288" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="288"/>
-      <c r="O2" s="288"/>
-      <c r="P2" s="288"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="294" t="s">
+      <c r="A3" s="290" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="294"/>
-      <c r="C3" s="294"/>
-      <c r="D3" s="294"/>
-      <c r="E3" s="294"/>
-      <c r="F3" s="294"/>
-      <c r="G3" s="294" t="s">
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="294"/>
-      <c r="I3" s="294"/>
-      <c r="J3" s="294"/>
-      <c r="K3" s="294"/>
-      <c r="L3" s="294"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="201" t="s">
         <v>303</v>
       </c>
@@ -9120,24 +9120,24 @@
       <c r="Q3" s="205"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="286"/>
-      <c r="C4" s="286"/>
-      <c r="D4" s="286" t="s">
+      <c r="B4" s="289"/>
+      <c r="C4" s="289"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="286"/>
-      <c r="I4" s="286"/>
-      <c r="J4" s="286"/>
-      <c r="K4" s="286"/>
-      <c r="L4" s="286"/>
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="166" t="s">
         <v>254</v>
       </c>
@@ -9152,12 +9152,12 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="287"/>
-      <c r="B5" s="287"/>
-      <c r="C5" s="287"/>
-      <c r="D5" s="287"/>
-      <c r="E5" s="287"/>
-      <c r="F5" s="287"/>
+      <c r="A5" s="286"/>
+      <c r="B5" s="286"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="286"/>
+      <c r="E5" s="286"/>
+      <c r="F5" s="286"/>
       <c r="G5" s="295" t="s">
         <v>4</v>
       </c>
@@ -9169,21 +9169,23 @@
       <c r="M5" s="200" t="s">
         <v>294</v>
       </c>
-      <c r="N5" s="200"/>
+      <c r="N5" s="200" t="s">
+        <v>499</v>
+      </c>
       <c r="O5" s="200" t="s">
         <v>395</v>
       </c>
       <c r="P5" s="200" t="s">
-        <v>396</v>
+        <v>465</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="287"/>
-      <c r="B6" s="287"/>
-      <c r="C6" s="287"/>
-      <c r="D6" s="287"/>
-      <c r="E6" s="287"/>
-      <c r="F6" s="287"/>
+      <c r="A6" s="286"/>
+      <c r="B6" s="286"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="286"/>
+      <c r="E6" s="286"/>
+      <c r="F6" s="286"/>
       <c r="G6" s="295"/>
       <c r="H6" s="295"/>
       <c r="I6" s="295"/>
@@ -9196,12 +9198,12 @@
       <c r="P6" s="167"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="287"/>
-      <c r="B7" s="287"/>
-      <c r="C7" s="287"/>
-      <c r="D7" s="287"/>
-      <c r="E7" s="287"/>
-      <c r="F7" s="287"/>
+      <c r="A7" s="286"/>
+      <c r="B7" s="286"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
       <c r="G7" s="295"/>
       <c r="H7" s="295"/>
       <c r="I7" s="295"/>
@@ -9214,12 +9216,12 @@
       <c r="P7" s="165"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="287"/>
-      <c r="B8" s="287"/>
-      <c r="C8" s="287"/>
-      <c r="D8" s="287"/>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
+      <c r="A8" s="286"/>
+      <c r="B8" s="286"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="286"/>
+      <c r="E8" s="286"/>
+      <c r="F8" s="286"/>
       <c r="G8" s="295"/>
       <c r="H8" s="295"/>
       <c r="I8" s="295"/>
@@ -9233,17 +9235,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="289" t="s">
+      <c r="A10" s="292" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="290"/>
-      <c r="C10" s="290"/>
-      <c r="D10" s="290"/>
-      <c r="E10" s="290"/>
-      <c r="F10" s="290"/>
-      <c r="G10" s="290"/>
-      <c r="H10" s="290"/>
-      <c r="I10" s="291"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="131" t="s">
@@ -9414,7 +9416,7 @@
         <v>317</v>
       </c>
       <c r="C23" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D23" s="180" t="s">
         <v>375</v>
@@ -9428,7 +9430,7 @@
         <v>342</v>
       </c>
       <c r="C24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D24" s="193" t="s">
         <v>339</v>
@@ -9442,7 +9444,7 @@
         <v>343</v>
       </c>
       <c r="C25" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D25" s="180" t="s">
         <v>340</v>
@@ -9456,7 +9458,7 @@
         <v>344</v>
       </c>
       <c r="C26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D26" s="180" t="s">
         <v>362</v>
@@ -9470,7 +9472,7 @@
         <v>345</v>
       </c>
       <c r="C27" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D27" s="183" t="s">
         <v>341</v>
@@ -9484,10 +9486,10 @@
         <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D28" s="193" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -9498,10 +9500,10 @@
         <v>318</v>
       </c>
       <c r="C29" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D29" s="193" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -9512,10 +9514,10 @@
         <v>318</v>
       </c>
       <c r="C30" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D30" s="193" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -9526,7 +9528,7 @@
         <v>318</v>
       </c>
       <c r="C31" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D31" s="193" t="s">
         <v>350</v>
@@ -9540,7 +9542,7 @@
         <v>346</v>
       </c>
       <c r="C32" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D32" s="193" t="s">
         <v>351</v>
@@ -9554,10 +9556,10 @@
         <v>384</v>
       </c>
       <c r="C33" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D33" s="180" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -9568,7 +9570,7 @@
         <v>353</v>
       </c>
       <c r="C34" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D34" s="193" t="s">
         <v>354</v>
@@ -9576,6 +9578,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9592,16 +9604,6 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9667,7 +9669,7 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -9772,10 +9774,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="214" t="s">
+        <v>495</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>496</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>497</v>
       </c>
       <c r="C7" s="215">
         <v>0</v>
@@ -9786,10 +9788,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="214" t="s">
+        <v>497</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>498</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>499</v>
       </c>
       <c r="C8" s="215">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed typo that tests detected
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -3937,20 +3937,116 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3973,102 +4069,6 @@
     <xf numFmtId="49" fontId="16" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4147,12 +4147,30 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4165,14 +4183,32 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="17" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4227,42 +4263,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5115,86 +5115,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="225" t="s">
+      <c r="A1" s="236" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="226"/>
-      <c r="C1" s="226"/>
-      <c r="D1" s="226"/>
-      <c r="E1" s="226"/>
-      <c r="F1" s="226"/>
-      <c r="G1" s="226"/>
-      <c r="H1" s="226"/>
-      <c r="I1" s="226"/>
-      <c r="J1" s="226"/>
-      <c r="K1" s="227"/>
+      <c r="B1" s="237"/>
+      <c r="C1" s="237"/>
+      <c r="D1" s="237"/>
+      <c r="E1" s="237"/>
+      <c r="F1" s="237"/>
+      <c r="G1" s="237"/>
+      <c r="H1" s="237"/>
+      <c r="I1" s="237"/>
+      <c r="J1" s="237"/>
+      <c r="K1" s="238"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="86"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="241" t="s">
+      <c r="A3" s="215" t="s">
         <v>321</v>
       </c>
-      <c r="B3" s="242"/>
+      <c r="B3" s="216"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="239" t="s">
+      <c r="A4" s="229" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="240"/>
+      <c r="B4" s="230"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="255" t="s">
+      <c r="A5" s="231" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="256"/>
+      <c r="B5" s="232"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="86"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="241" t="s">
+      <c r="A7" s="215" t="s">
         <v>276</v>
       </c>
-      <c r="B7" s="243"/>
-      <c r="C7" s="243"/>
-      <c r="D7" s="243"/>
-      <c r="E7" s="243"/>
-      <c r="F7" s="243"/>
-      <c r="G7" s="243"/>
-      <c r="H7" s="243"/>
-      <c r="I7" s="243"/>
-      <c r="J7" s="243"/>
-      <c r="K7" s="242"/>
+      <c r="B7" s="217"/>
+      <c r="C7" s="217"/>
+      <c r="D7" s="217"/>
+      <c r="E7" s="217"/>
+      <c r="F7" s="217"/>
+      <c r="G7" s="217"/>
+      <c r="H7" s="217"/>
+      <c r="I7" s="217"/>
+      <c r="J7" s="217"/>
+      <c r="K7" s="216"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="228" t="s">
+      <c r="A8" s="239" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="229"/>
-      <c r="C8" s="229"/>
-      <c r="D8" s="229"/>
-      <c r="E8" s="229"/>
-      <c r="F8" s="229"/>
-      <c r="G8" s="229"/>
-      <c r="H8" s="229"/>
-      <c r="I8" s="229"/>
-      <c r="J8" s="229"/>
-      <c r="K8" s="230"/>
+      <c r="B8" s="240"/>
+      <c r="C8" s="240"/>
+      <c r="D8" s="240"/>
+      <c r="E8" s="240"/>
+      <c r="F8" s="240"/>
+      <c r="G8" s="240"/>
+      <c r="H8" s="240"/>
+      <c r="I8" s="240"/>
+      <c r="J8" s="240"/>
+      <c r="K8" s="241"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="231"/>
-      <c r="B9" s="232"/>
-      <c r="C9" s="232"/>
-      <c r="D9" s="232"/>
-      <c r="E9" s="232"/>
-      <c r="F9" s="232"/>
-      <c r="G9" s="232"/>
-      <c r="H9" s="232"/>
-      <c r="I9" s="232"/>
-      <c r="J9" s="232"/>
-      <c r="K9" s="233"/>
+      <c r="A9" s="242"/>
+      <c r="B9" s="243"/>
+      <c r="C9" s="243"/>
+      <c r="D9" s="243"/>
+      <c r="E9" s="243"/>
+      <c r="F9" s="243"/>
+      <c r="G9" s="243"/>
+      <c r="H9" s="243"/>
+      <c r="I9" s="243"/>
+      <c r="J9" s="243"/>
+      <c r="K9" s="244"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="156"/>
@@ -5205,62 +5205,62 @@
       <c r="F10" s="142"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="244" t="s">
+      <c r="A11" s="218" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="245"/>
-      <c r="C11" s="245"/>
-      <c r="D11" s="246"/>
+      <c r="B11" s="219"/>
+      <c r="C11" s="219"/>
+      <c r="D11" s="220"/>
       <c r="E11" s="87"/>
       <c r="F11" s="142"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="247" t="s">
+      <c r="A12" s="221" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="248"/>
-      <c r="C12" s="249" t="s">
+      <c r="B12" s="222"/>
+      <c r="C12" s="223" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="250"/>
+      <c r="D12" s="224"/>
       <c r="E12" s="87"/>
       <c r="F12" s="142"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="251"/>
-      <c r="B13" s="252"/>
-      <c r="C13" s="253"/>
-      <c r="D13" s="254"/>
+      <c r="A13" s="225"/>
+      <c r="B13" s="226"/>
+      <c r="C13" s="227"/>
+      <c r="D13" s="228"/>
       <c r="E13" s="87"/>
       <c r="F13" s="142"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="244" t="s">
+      <c r="A15" s="218" t="s">
         <v>278</v>
       </c>
-      <c r="B15" s="246"/>
-      <c r="E15" s="244" t="s">
+      <c r="B15" s="220"/>
+      <c r="E15" s="218" t="s">
         <v>320</v>
       </c>
-      <c r="F15" s="245"/>
-      <c r="G15" s="245"/>
-      <c r="H15" s="245"/>
-      <c r="I15" s="246"/>
+      <c r="F15" s="219"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="220"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="239" t="s">
+      <c r="A16" s="229" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="240"/>
+      <c r="B16" s="230"/>
       <c r="D16" s="88"/>
-      <c r="E16" s="234" t="s">
+      <c r="E16" s="245" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="235"/>
-      <c r="G16" s="235"/>
-      <c r="H16" s="235"/>
-      <c r="I16" s="236"/>
+      <c r="F16" s="246"/>
+      <c r="G16" s="246"/>
+      <c r="H16" s="246"/>
+      <c r="I16" s="247"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="157" t="s">
@@ -5270,10 +5270,10 @@
         <v>281</v>
       </c>
       <c r="C17" s="89"/>
-      <c r="E17" s="237" t="s">
+      <c r="E17" s="248" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="238"/>
+      <c r="F17" s="249"/>
       <c r="G17" s="210" t="s">
         <v>159</v>
       </c>
@@ -5303,7 +5303,7 @@
       <c r="H18" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="213" t="s">
+      <c r="I18" s="233" t="s">
         <v>491</v>
       </c>
       <c r="J18" s="81"/>
@@ -5326,7 +5326,7 @@
       <c r="H19" s="74" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="213"/>
+      <c r="I19" s="233"/>
       <c r="J19" s="81"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5343,7 +5343,7 @@
       </c>
       <c r="G20" s="71"/>
       <c r="H20" s="71"/>
-      <c r="I20" s="214"/>
+      <c r="I20" s="234"/>
       <c r="J20" s="81"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5365,24 +5365,24 @@
       <c r="A23" s="161"/>
       <c r="B23" s="92"/>
       <c r="C23" s="91"/>
-      <c r="E23" s="215" t="s">
+      <c r="E23" s="213" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="216"/>
-      <c r="G23" s="216"/>
-      <c r="H23" s="216"/>
-      <c r="I23" s="217"/>
+      <c r="F23" s="235"/>
+      <c r="G23" s="235"/>
+      <c r="H23" s="235"/>
+      <c r="I23" s="214"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="215" t="s">
+      <c r="A24" s="213" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="217"/>
+      <c r="B24" s="214"/>
       <c r="C24" s="32"/>
-      <c r="E24" s="221" t="s">
+      <c r="E24" s="253" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="222"/>
+      <c r="F24" s="254"/>
       <c r="G24" s="210" t="s">
         <v>159</v>
       </c>
@@ -5411,7 +5411,7 @@
       <c r="H25" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="218" t="s">
+      <c r="I25" s="250" t="s">
         <v>492</v>
       </c>
     </row>
@@ -5435,7 +5435,7 @@
       <c r="H26" s="74" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="219"/>
+      <c r="I26" s="251"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="159" t="s">
@@ -5451,7 +5451,7 @@
       </c>
       <c r="G27" s="71"/>
       <c r="H27" s="71"/>
-      <c r="I27" s="220"/>
+      <c r="I27" s="252"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="159" t="s">
@@ -5475,22 +5475,22 @@
       <c r="A30" s="160"/>
       <c r="B30" s="117"/>
       <c r="C30" s="89"/>
-      <c r="E30" s="215" t="s">
+      <c r="E30" s="213" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="216"/>
-      <c r="G30" s="216"/>
-      <c r="H30" s="216"/>
-      <c r="I30" s="217"/>
+      <c r="F30" s="235"/>
+      <c r="G30" s="235"/>
+      <c r="H30" s="235"/>
+      <c r="I30" s="214"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="161"/>
       <c r="B31" s="91"/>
       <c r="C31" s="91"/>
-      <c r="E31" s="223" t="s">
+      <c r="E31" s="255" t="s">
         <v>469</v>
       </c>
-      <c r="F31" s="224"/>
+      <c r="F31" s="256"/>
       <c r="G31" s="208" t="s">
         <v>159</v>
       </c>
@@ -5502,10 +5502,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="215" t="s">
+      <c r="A32" s="213" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="217"/>
+      <c r="B32" s="214"/>
       <c r="C32" s="32"/>
       <c r="E32" s="83">
         <v>1</v>
@@ -5515,7 +5515,7 @@
       </c>
       <c r="G32" s="33"/>
       <c r="H32" s="74"/>
-      <c r="I32" s="213"/>
+      <c r="I32" s="233"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="157" t="s">
@@ -5535,7 +5535,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="33"/>
-      <c r="I33" s="213"/>
+      <c r="I33" s="233"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="158" t="s">
@@ -5550,7 +5550,7 @@
       <c r="F34" s="93"/>
       <c r="G34" s="33"/>
       <c r="H34" s="74"/>
-      <c r="I34" s="213"/>
+      <c r="I34" s="233"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="159" t="s">
@@ -5563,7 +5563,7 @@
       <c r="F35" s="93"/>
       <c r="G35" s="33"/>
       <c r="H35" s="33"/>
-      <c r="I35" s="213"/>
+      <c r="I35" s="233"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="159" t="s">
@@ -5576,7 +5576,7 @@
       <c r="F36" s="93"/>
       <c r="G36" s="33"/>
       <c r="H36" s="33"/>
-      <c r="I36" s="213"/>
+      <c r="I36" s="233"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="159" t="s">
@@ -5589,7 +5589,7 @@
       <c r="F37" s="140"/>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
-      <c r="I37" s="214"/>
+      <c r="I37" s="234"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="160" t="s">
@@ -5602,17 +5602,17 @@
       <c r="B39" s="121"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="215" t="s">
+      <c r="E40" s="213" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="216"/>
-      <c r="G40" s="216"/>
-      <c r="H40" s="216"/>
-      <c r="I40" s="217"/>
+      <c r="F40" s="235"/>
+      <c r="G40" s="235"/>
+      <c r="H40" s="235"/>
+      <c r="I40" s="214"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="221"/>
-      <c r="F41" s="222"/>
+      <c r="E41" s="253"/>
+      <c r="F41" s="254"/>
       <c r="G41" s="82" t="s">
         <v>159</v>
       </c>
@@ -5630,7 +5630,7 @@
       <c r="F42" s="93"/>
       <c r="G42" s="33"/>
       <c r="H42" s="74"/>
-      <c r="I42" s="213"/>
+      <c r="I42" s="233"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="83">
@@ -5639,7 +5639,7 @@
       <c r="F43" s="93"/>
       <c r="G43" s="33"/>
       <c r="H43" s="33"/>
-      <c r="I43" s="213"/>
+      <c r="I43" s="233"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="83">
@@ -5648,7 +5648,7 @@
       <c r="F44" s="93"/>
       <c r="G44" s="33"/>
       <c r="H44" s="74"/>
-      <c r="I44" s="213"/>
+      <c r="I44" s="233"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="83">
@@ -5657,7 +5657,7 @@
       <c r="F45" s="93"/>
       <c r="G45" s="33"/>
       <c r="H45" s="33"/>
-      <c r="I45" s="213"/>
+      <c r="I45" s="233"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="83">
@@ -5666,7 +5666,7 @@
       <c r="F46" s="93"/>
       <c r="G46" s="33"/>
       <c r="H46" s="33"/>
-      <c r="I46" s="213"/>
+      <c r="I46" s="233"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="84">
@@ -5675,11 +5675,25 @@
       <c r="F47" s="140"/>
       <c r="G47" s="71"/>
       <c r="H47" s="71"/>
-      <c r="I47" s="214"/>
+      <c r="I47" s="234"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -5695,20 +5709,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8076,7 +8076,7 @@
   </sheetPr>
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:C7"/>
     </sheetView>
   </sheetViews>
@@ -8102,68 +8102,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="289" t="s">
+      <c r="A1" s="287" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="289"/>
-      <c r="C1" s="289"/>
-      <c r="D1" s="289"/>
-      <c r="E1" s="289"/>
-      <c r="F1" s="289"/>
-      <c r="G1" s="289"/>
-      <c r="H1" s="289"/>
-      <c r="I1" s="289"/>
-      <c r="J1" s="289"/>
-      <c r="K1" s="289"/>
-      <c r="L1" s="289"/>
-      <c r="M1" s="289"/>
-      <c r="N1" s="289"/>
-      <c r="O1" s="289"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="309" t="s">
+      <c r="A2" s="295" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="310"/>
-      <c r="C2" s="310"/>
-      <c r="D2" s="310"/>
-      <c r="E2" s="310"/>
-      <c r="F2" s="311"/>
-      <c r="G2" s="290" t="s">
+      <c r="B2" s="296"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="297"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="290"/>
-      <c r="I2" s="290"/>
-      <c r="J2" s="290"/>
-      <c r="K2" s="290"/>
-      <c r="L2" s="290"/>
-      <c r="M2" s="285" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>299</v>
       </c>
-      <c r="N2" s="285"/>
-      <c r="O2" s="285"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
       <c r="P2" s="88"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="312" t="s">
+      <c r="A3" s="298" t="s">
         <v>298</v>
       </c>
-      <c r="B3" s="313"/>
-      <c r="C3" s="313"/>
-      <c r="D3" s="313"/>
-      <c r="E3" s="313"/>
-      <c r="F3" s="314"/>
-      <c r="G3" s="291" t="s">
+      <c r="B3" s="299"/>
+      <c r="C3" s="299"/>
+      <c r="D3" s="299"/>
+      <c r="E3" s="299"/>
+      <c r="F3" s="300"/>
+      <c r="G3" s="290" t="s">
         <v>306</v>
       </c>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="200" t="s">
         <v>304</v>
       </c>
@@ -8176,26 +8176,26 @@
       <c r="P3" s="203"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="315" t="s">
+      <c r="A4" s="301" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="316"/>
-      <c r="C4" s="317"/>
-      <c r="D4" s="283" t="s">
+      <c r="B4" s="302"/>
+      <c r="C4" s="303"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="283"/>
-      <c r="F4" s="283"/>
-      <c r="G4" s="283" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="283"/>
-      <c r="I4" s="283"/>
-      <c r="J4" s="283" t="s">
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289" t="s">
         <v>307</v>
       </c>
-      <c r="K4" s="283"/>
-      <c r="L4" s="283"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="166" t="s">
         <v>154</v>
       </c>
@@ -8207,22 +8207,22 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="318"/>
-      <c r="B5" s="319"/>
-      <c r="C5" s="320"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284" t="s">
+      <c r="A5" s="284"/>
+      <c r="B5" s="285"/>
+      <c r="C5" s="286"/>
+      <c r="D5" s="283"/>
+      <c r="E5" s="283"/>
+      <c r="F5" s="283"/>
+      <c r="G5" s="283" t="s">
         <v>281</v>
       </c>
-      <c r="H5" s="284"/>
-      <c r="I5" s="284"/>
-      <c r="J5" s="284" t="s">
+      <c r="H5" s="283"/>
+      <c r="I5" s="283"/>
+      <c r="J5" s="283" t="s">
         <v>295</v>
       </c>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
+      <c r="K5" s="283"/>
+      <c r="L5" s="283"/>
       <c r="M5" s="199"/>
       <c r="N5" s="199" t="s">
         <v>389</v>
@@ -8232,24 +8232,24 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="318" t="s">
+      <c r="A6" s="284" t="s">
         <v>281</v>
       </c>
-      <c r="B6" s="319"/>
-      <c r="C6" s="320"/>
-      <c r="D6" s="284" t="s">
+      <c r="B6" s="285"/>
+      <c r="C6" s="286"/>
+      <c r="D6" s="283" t="s">
         <v>291</v>
       </c>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="284" t="s">
+      <c r="E6" s="283"/>
+      <c r="F6" s="283"/>
+      <c r="G6" s="283" t="s">
         <v>288</v>
       </c>
-      <c r="H6" s="284"/>
-      <c r="I6" s="284"/>
-      <c r="J6" s="284"/>
-      <c r="K6" s="284"/>
-      <c r="L6" s="284"/>
+      <c r="H6" s="283"/>
+      <c r="I6" s="283"/>
+      <c r="J6" s="283"/>
+      <c r="K6" s="283"/>
+      <c r="L6" s="283"/>
       <c r="M6" s="199"/>
       <c r="N6" s="199" t="s">
         <v>390</v>
@@ -8259,58 +8259,58 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="318" t="s">
+      <c r="A7" s="284" t="s">
         <v>281</v>
       </c>
-      <c r="B7" s="319"/>
-      <c r="C7" s="320"/>
-      <c r="D7" s="284" t="s">
+      <c r="B7" s="285"/>
+      <c r="C7" s="286"/>
+      <c r="D7" s="283" t="s">
         <v>292</v>
       </c>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
-      <c r="H7" s="284"/>
-      <c r="I7" s="284"/>
-      <c r="J7" s="284"/>
-      <c r="K7" s="284"/>
-      <c r="L7" s="284"/>
+      <c r="E7" s="283"/>
+      <c r="F7" s="283"/>
+      <c r="G7" s="283"/>
+      <c r="H7" s="283"/>
+      <c r="I7" s="283"/>
+      <c r="J7" s="283"/>
+      <c r="K7" s="283"/>
+      <c r="L7" s="283"/>
       <c r="M7" s="199"/>
       <c r="N7" s="199"/>
       <c r="O7" s="164"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="318"/>
-      <c r="B8" s="319"/>
-      <c r="C8" s="320"/>
-      <c r="D8" s="284" t="s">
+      <c r="A8" s="284"/>
+      <c r="B8" s="285"/>
+      <c r="C8" s="286"/>
+      <c r="D8" s="283" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="284"/>
-      <c r="H8" s="284"/>
-      <c r="I8" s="284"/>
-      <c r="J8" s="284"/>
-      <c r="K8" s="284"/>
-      <c r="L8" s="284"/>
+      <c r="E8" s="283"/>
+      <c r="F8" s="283"/>
+      <c r="G8" s="283"/>
+      <c r="H8" s="283"/>
+      <c r="I8" s="283"/>
+      <c r="J8" s="283"/>
+      <c r="K8" s="283"/>
+      <c r="L8" s="283"/>
       <c r="M8" s="199"/>
       <c r="N8" s="199"/>
       <c r="O8" s="164"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="286" t="s">
+      <c r="A10" s="292" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="287"/>
-      <c r="C10" s="287"/>
-      <c r="D10" s="287"/>
-      <c r="E10" s="287"/>
-      <c r="F10" s="287"/>
-      <c r="G10" s="287"/>
-      <c r="H10" s="287"/>
-      <c r="I10" s="288"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="131" t="s">
@@ -8910,13 +8910,18 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -8929,18 +8934,13 @@
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="D4:F4"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9032,68 +9032,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="289" t="s">
+      <c r="A1" s="287" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="289"/>
-      <c r="C1" s="289"/>
-      <c r="D1" s="289"/>
-      <c r="E1" s="289"/>
-      <c r="F1" s="289"/>
-      <c r="G1" s="289"/>
-      <c r="H1" s="289"/>
-      <c r="I1" s="289"/>
-      <c r="J1" s="289"/>
-      <c r="K1" s="289"/>
-      <c r="L1" s="289"/>
-      <c r="M1" s="289"/>
-      <c r="N1" s="289"/>
-      <c r="O1" s="289"/>
-      <c r="P1" s="289"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
+      <c r="L1" s="287"/>
+      <c r="M1" s="287"/>
+      <c r="N1" s="287"/>
+      <c r="O1" s="287"/>
+      <c r="P1" s="287"/>
       <c r="Q1" s="31"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="290" t="s">
+      <c r="A2" s="288" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="290"/>
-      <c r="C2" s="290"/>
-      <c r="D2" s="290"/>
-      <c r="E2" s="290"/>
-      <c r="F2" s="290"/>
-      <c r="G2" s="290" t="s">
+      <c r="B2" s="288"/>
+      <c r="C2" s="288"/>
+      <c r="D2" s="288"/>
+      <c r="E2" s="288"/>
+      <c r="F2" s="288"/>
+      <c r="G2" s="288" t="s">
         <v>248</v>
       </c>
-      <c r="H2" s="290"/>
-      <c r="I2" s="290"/>
-      <c r="J2" s="290"/>
-      <c r="K2" s="290"/>
-      <c r="L2" s="290"/>
-      <c r="M2" s="285" t="s">
+      <c r="H2" s="288"/>
+      <c r="I2" s="288"/>
+      <c r="J2" s="288"/>
+      <c r="K2" s="288"/>
+      <c r="L2" s="288"/>
+      <c r="M2" s="291" t="s">
         <v>297</v>
       </c>
-      <c r="N2" s="285"/>
-      <c r="O2" s="285"/>
-      <c r="P2" s="285"/>
+      <c r="N2" s="291"/>
+      <c r="O2" s="291"/>
+      <c r="P2" s="291"/>
       <c r="Q2" s="88"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="291" t="s">
+      <c r="A3" s="290" t="s">
         <v>301</v>
       </c>
-      <c r="B3" s="291"/>
-      <c r="C3" s="291"/>
-      <c r="D3" s="291"/>
-      <c r="E3" s="291"/>
-      <c r="F3" s="291"/>
-      <c r="G3" s="291" t="s">
+      <c r="B3" s="290"/>
+      <c r="C3" s="290"/>
+      <c r="D3" s="290"/>
+      <c r="E3" s="290"/>
+      <c r="F3" s="290"/>
+      <c r="G3" s="290" t="s">
         <v>300</v>
       </c>
-      <c r="H3" s="291"/>
-      <c r="I3" s="291"/>
-      <c r="J3" s="291"/>
-      <c r="K3" s="291"/>
-      <c r="L3" s="291"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="290"/>
+      <c r="J3" s="290"/>
+      <c r="K3" s="290"/>
+      <c r="L3" s="290"/>
       <c r="M3" s="200" t="s">
         <v>303</v>
       </c>
@@ -9109,24 +9109,24 @@
       <c r="Q3" s="202"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="283" t="s">
+      <c r="A4" s="289" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="283"/>
-      <c r="C4" s="283"/>
-      <c r="D4" s="283" t="s">
+      <c r="B4" s="289"/>
+      <c r="C4" s="289"/>
+      <c r="D4" s="289" t="s">
         <v>247</v>
       </c>
-      <c r="E4" s="283"/>
-      <c r="F4" s="283"/>
-      <c r="G4" s="283" t="s">
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289" t="s">
         <v>250</v>
       </c>
-      <c r="H4" s="283"/>
-      <c r="I4" s="283"/>
-      <c r="J4" s="283"/>
-      <c r="K4" s="283"/>
-      <c r="L4" s="283"/>
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
       <c r="M4" s="166" t="s">
         <v>254</v>
       </c>
@@ -9141,20 +9141,20 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="284"/>
-      <c r="B5" s="284"/>
-      <c r="C5" s="284"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="292" t="s">
+      <c r="A5" s="283"/>
+      <c r="B5" s="283"/>
+      <c r="C5" s="283"/>
+      <c r="D5" s="283"/>
+      <c r="E5" s="283"/>
+      <c r="F5" s="283"/>
+      <c r="G5" s="304" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="292"/>
-      <c r="I5" s="292"/>
-      <c r="J5" s="292"/>
-      <c r="K5" s="292"/>
-      <c r="L5" s="292"/>
+      <c r="H5" s="304"/>
+      <c r="I5" s="304"/>
+      <c r="J5" s="304"/>
+      <c r="K5" s="304"/>
+      <c r="L5" s="304"/>
       <c r="M5" s="199" t="s">
         <v>294</v>
       </c>
@@ -9169,54 +9169,54 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="284"/>
-      <c r="B6" s="284"/>
-      <c r="C6" s="284"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="292"/>
-      <c r="H6" s="292"/>
-      <c r="I6" s="292"/>
-      <c r="J6" s="292"/>
-      <c r="K6" s="292"/>
-      <c r="L6" s="292"/>
+      <c r="A6" s="283"/>
+      <c r="B6" s="283"/>
+      <c r="C6" s="283"/>
+      <c r="D6" s="283"/>
+      <c r="E6" s="283"/>
+      <c r="F6" s="283"/>
+      <c r="G6" s="304"/>
+      <c r="H6" s="304"/>
+      <c r="I6" s="304"/>
+      <c r="J6" s="304"/>
+      <c r="K6" s="304"/>
+      <c r="L6" s="304"/>
       <c r="M6" s="199"/>
       <c r="N6" s="199"/>
       <c r="O6" s="199"/>
       <c r="P6" s="167"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="284"/>
-      <c r="B7" s="284"/>
-      <c r="C7" s="284"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="292"/>
-      <c r="H7" s="292"/>
-      <c r="I7" s="292"/>
-      <c r="J7" s="292"/>
-      <c r="K7" s="292"/>
-      <c r="L7" s="292"/>
+      <c r="A7" s="283"/>
+      <c r="B7" s="283"/>
+      <c r="C7" s="283"/>
+      <c r="D7" s="283"/>
+      <c r="E7" s="283"/>
+      <c r="F7" s="283"/>
+      <c r="G7" s="304"/>
+      <c r="H7" s="304"/>
+      <c r="I7" s="304"/>
+      <c r="J7" s="304"/>
+      <c r="K7" s="304"/>
+      <c r="L7" s="304"/>
       <c r="M7" s="199"/>
       <c r="N7" s="199"/>
       <c r="O7" s="199"/>
       <c r="P7" s="165"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="284"/>
-      <c r="B8" s="284"/>
-      <c r="C8" s="284"/>
-      <c r="D8" s="284"/>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="292"/>
-      <c r="H8" s="292"/>
-      <c r="I8" s="292"/>
-      <c r="J8" s="292"/>
-      <c r="K8" s="292"/>
-      <c r="L8" s="292"/>
+      <c r="A8" s="283"/>
+      <c r="B8" s="283"/>
+      <c r="C8" s="283"/>
+      <c r="D8" s="283"/>
+      <c r="E8" s="283"/>
+      <c r="F8" s="283"/>
+      <c r="G8" s="304"/>
+      <c r="H8" s="304"/>
+      <c r="I8" s="304"/>
+      <c r="J8" s="304"/>
+      <c r="K8" s="304"/>
+      <c r="L8" s="304"/>
       <c r="M8" s="199"/>
       <c r="N8" s="199"/>
       <c r="O8" s="199"/>
@@ -9224,17 +9224,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="286" t="s">
+      <c r="A10" s="292" t="s">
         <v>358</v>
       </c>
-      <c r="B10" s="287"/>
-      <c r="C10" s="287"/>
-      <c r="D10" s="287"/>
-      <c r="E10" s="287"/>
-      <c r="F10" s="287"/>
-      <c r="G10" s="287"/>
-      <c r="H10" s="287"/>
-      <c r="I10" s="288"/>
+      <c r="B10" s="293"/>
+      <c r="C10" s="293"/>
+      <c r="D10" s="293"/>
+      <c r="E10" s="293"/>
+      <c r="F10" s="293"/>
+      <c r="G10" s="293"/>
+      <c r="H10" s="293"/>
+      <c r="I10" s="294"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="131" t="s">
@@ -9567,6 +9567,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
     <mergeCell ref="D22:G22"/>
@@ -9583,16 +9593,6 @@
     <mergeCell ref="G7:L7"/>
     <mergeCell ref="G8:L8"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9658,8 +9658,8 @@
   </sheetPr>
   <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9674,12 +9674,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="293" t="s">
+      <c r="A1" s="305" t="s">
         <v>251</v>
       </c>
-      <c r="B1" s="294"/>
-      <c r="C1" s="294"/>
-      <c r="D1" s="295"/>
+      <c r="B1" s="306"/>
+      <c r="C1" s="306"/>
+      <c r="D1" s="307"/>
       <c r="E1" s="66"/>
       <c r="F1" s="66"/>
       <c r="G1" s="66"/>
@@ -9754,9 +9754,7 @@
       <c r="B6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="187">
-        <v>1</v>
-      </c>
+      <c r="C6" s="187"/>
       <c r="D6" s="24">
         <v>0</v>
       </c>
@@ -10444,23 +10442,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="299" t="s">
+      <c r="A1" s="311" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="300"/>
-      <c r="C1" s="300"/>
-      <c r="D1" s="300"/>
-      <c r="E1" s="300"/>
-      <c r="F1" s="300"/>
-      <c r="G1" s="300"/>
-      <c r="H1" s="300"/>
-      <c r="I1" s="300"/>
-      <c r="J1" s="300"/>
-      <c r="K1" s="300"/>
-      <c r="L1" s="300"/>
-      <c r="M1" s="300"/>
-      <c r="N1" s="300"/>
-      <c r="O1" s="300"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
+      <c r="H1" s="312"/>
+      <c r="I1" s="312"/>
+      <c r="J1" s="312"/>
+      <c r="K1" s="312"/>
+      <c r="L1" s="312"/>
+      <c r="M1" s="312"/>
+      <c r="N1" s="312"/>
+      <c r="O1" s="312"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -10478,17 +10476,17 @@
       <c r="M2" s="35"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="296" t="s">
+      <c r="B3" s="308" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="297"/>
-      <c r="D3" s="297"/>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="297"/>
-      <c r="I3" s="297"/>
-      <c r="J3" s="298"/>
+      <c r="C3" s="309"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="309"/>
+      <c r="H3" s="309"/>
+      <c r="I3" s="309"/>
+      <c r="J3" s="310"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="37"/>
@@ -10679,21 +10677,21 @@
     </row>
     <row r="18" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="296" t="s">
+      <c r="B19" s="308" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="297"/>
-      <c r="D19" s="297"/>
-      <c r="E19" s="297"/>
-      <c r="F19" s="297"/>
-      <c r="G19" s="297"/>
-      <c r="H19" s="297"/>
-      <c r="I19" s="297"/>
-      <c r="J19" s="297"/>
-      <c r="K19" s="297"/>
-      <c r="L19" s="297"/>
-      <c r="M19" s="297"/>
-      <c r="N19" s="298"/>
+      <c r="C19" s="309"/>
+      <c r="D19" s="309"/>
+      <c r="E19" s="309"/>
+      <c r="F19" s="309"/>
+      <c r="G19" s="309"/>
+      <c r="H19" s="309"/>
+      <c r="I19" s="309"/>
+      <c r="J19" s="309"/>
+      <c r="K19" s="309"/>
+      <c r="L19" s="309"/>
+      <c r="M19" s="309"/>
+      <c r="N19" s="310"/>
     </row>
     <row r="20" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="37"/>
@@ -10895,27 +10893,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="304" t="s">
+      <c r="A1" s="316" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="305"/>
-      <c r="C1" s="305"/>
-      <c r="D1" s="305"/>
-      <c r="E1" s="305"/>
-      <c r="F1" s="305"/>
-      <c r="G1" s="305"/>
-      <c r="H1" s="305"/>
-      <c r="I1" s="305"/>
-      <c r="J1" s="305"/>
-      <c r="K1" s="305"/>
-      <c r="L1" s="305"/>
-      <c r="M1" s="305"/>
-      <c r="N1" s="305"/>
-      <c r="O1" s="305"/>
-      <c r="P1" s="305"/>
-      <c r="Q1" s="305"/>
-      <c r="R1" s="305"/>
-      <c r="S1" s="305"/>
+      <c r="B1" s="317"/>
+      <c r="C1" s="317"/>
+      <c r="D1" s="317"/>
+      <c r="E1" s="317"/>
+      <c r="F1" s="317"/>
+      <c r="G1" s="317"/>
+      <c r="H1" s="317"/>
+      <c r="I1" s="317"/>
+      <c r="J1" s="317"/>
+      <c r="K1" s="317"/>
+      <c r="L1" s="317"/>
+      <c r="M1" s="317"/>
+      <c r="N1" s="317"/>
+      <c r="O1" s="317"/>
+      <c r="P1" s="317"/>
+      <c r="Q1" s="317"/>
+      <c r="R1" s="317"/>
+      <c r="S1" s="317"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="35"/>
@@ -10929,26 +10927,26 @@
       <c r="I2" s="35"/>
     </row>
     <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="296" t="s">
+      <c r="B3" s="308" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="297"/>
-      <c r="D3" s="297"/>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="297"/>
-      <c r="I3" s="297"/>
-      <c r="J3" s="298"/>
-      <c r="L3" s="301" t="s">
+      <c r="C3" s="309"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="309"/>
+      <c r="H3" s="309"/>
+      <c r="I3" s="309"/>
+      <c r="J3" s="310"/>
+      <c r="L3" s="313" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="302"/>
-      <c r="N3" s="302"/>
-      <c r="O3" s="302"/>
-      <c r="P3" s="302"/>
-      <c r="Q3" s="302"/>
-      <c r="R3" s="303"/>
+      <c r="M3" s="314"/>
+      <c r="N3" s="314"/>
+      <c r="O3" s="314"/>
+      <c r="P3" s="314"/>
+      <c r="Q3" s="314"/>
+      <c r="R3" s="315"/>
       <c r="S3" s="36"/>
       <c r="T3" s="36"/>
     </row>
@@ -11179,23 +11177,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="318" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="307"/>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="307"/>
-      <c r="G1" s="307"/>
-      <c r="H1" s="307"/>
-      <c r="I1" s="307"/>
-      <c r="J1" s="307"/>
-      <c r="K1" s="307"/>
-      <c r="L1" s="307"/>
-      <c r="M1" s="307"/>
-      <c r="N1" s="307"/>
-      <c r="O1" s="308"/>
+      <c r="B1" s="319"/>
+      <c r="C1" s="319"/>
+      <c r="D1" s="319"/>
+      <c r="E1" s="319"/>
+      <c r="F1" s="319"/>
+      <c r="G1" s="319"/>
+      <c r="H1" s="319"/>
+      <c r="I1" s="319"/>
+      <c r="J1" s="319"/>
+      <c r="K1" s="319"/>
+      <c r="L1" s="319"/>
+      <c r="M1" s="319"/>
+      <c r="N1" s="319"/>
+      <c r="O1" s="320"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -11208,22 +11206,22 @@
       <c r="H2" s="52"/>
     </row>
     <row r="3" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="296" t="s">
+      <c r="B3" s="308" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="297"/>
-      <c r="D3" s="297"/>
-      <c r="E3" s="297"/>
-      <c r="F3" s="297"/>
-      <c r="G3" s="297"/>
-      <c r="H3" s="298"/>
-      <c r="J3" s="301" t="s">
+      <c r="C3" s="309"/>
+      <c r="D3" s="309"/>
+      <c r="E3" s="309"/>
+      <c r="F3" s="309"/>
+      <c r="G3" s="309"/>
+      <c r="H3" s="310"/>
+      <c r="J3" s="313" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="302"/>
-      <c r="L3" s="302"/>
-      <c r="M3" s="302"/>
-      <c r="N3" s="303"/>
+      <c r="K3" s="314"/>
+      <c r="L3" s="314"/>
+      <c r="M3" s="314"/>
+      <c r="N3" s="315"/>
       <c r="O3" s="36"/>
       <c r="P3" s="36"/>
     </row>

</xml_diff>

<commit_message>
Fixed batch analysis octave bug
</commit_message>
<xml_diff>
--- a/test_templates/test_batch_template1.xlsx
+++ b/test_templates/test_batch_template1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="-50385" yWindow="1080" windowWidth="47745" windowHeight="25665" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1029" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="553">
   <si>
     <t>blank plasmid</t>
   </si>
@@ -2674,6 +2674,9 @@
   </si>
   <si>
     <t>When true, controls the random seed for GMM Gating</t>
+  </si>
+  <si>
+    <t>10^4</t>
   </si>
 </sst>
 </file>
@@ -4286,20 +4289,147 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4322,102 +4452,6 @@
     <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4477,6 +4511,12 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4509,57 +4549,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4572,6 +4561,57 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="16" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -4629,43 +4669,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4756,7 +4759,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4822,7 +4825,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4893,7 +4896,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -4964,7 +4967,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5030,7 +5033,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5101,7 +5104,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5167,7 +5170,7 @@
             </a:ln>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="ctr" rtl="0">
@@ -5497,7 +5500,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5518,86 +5521,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="251" t="s">
+      <c r="A1" s="271" t="s">
         <v>378</v>
       </c>
-      <c r="B1" s="252"/>
-      <c r="C1" s="252"/>
-      <c r="D1" s="252"/>
-      <c r="E1" s="252"/>
-      <c r="F1" s="252"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="252"/>
-      <c r="I1" s="252"/>
-      <c r="J1" s="252"/>
-      <c r="K1" s="253"/>
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="273"/>
     </row>
     <row r="2" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="85"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="267" t="s">
+      <c r="A3" s="250" t="s">
         <v>316</v>
       </c>
-      <c r="B3" s="268"/>
+      <c r="B3" s="251"/>
     </row>
     <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="264" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="266"/>
+      <c r="B4" s="265"/>
     </row>
     <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="281" t="s">
+      <c r="A5" s="266" t="s">
         <v>182</v>
       </c>
-      <c r="B5" s="282"/>
+      <c r="B5" s="267"/>
     </row>
     <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="85"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="267" t="s">
+      <c r="A7" s="250" t="s">
         <v>273</v>
       </c>
-      <c r="B7" s="269"/>
-      <c r="C7" s="269"/>
-      <c r="D7" s="269"/>
-      <c r="E7" s="269"/>
-      <c r="F7" s="269"/>
-      <c r="G7" s="269"/>
-      <c r="H7" s="269"/>
-      <c r="I7" s="269"/>
-      <c r="J7" s="269"/>
-      <c r="K7" s="268"/>
+      <c r="B7" s="252"/>
+      <c r="C7" s="252"/>
+      <c r="D7" s="252"/>
+      <c r="E7" s="252"/>
+      <c r="F7" s="252"/>
+      <c r="G7" s="252"/>
+      <c r="H7" s="252"/>
+      <c r="I7" s="252"/>
+      <c r="J7" s="252"/>
+      <c r="K7" s="251"/>
     </row>
     <row r="8" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="254" t="s">
+      <c r="A8" s="274" t="s">
         <v>162</v>
       </c>
-      <c r="B8" s="255"/>
-      <c r="C8" s="255"/>
-      <c r="D8" s="255"/>
-      <c r="E8" s="255"/>
-      <c r="F8" s="255"/>
-      <c r="G8" s="255"/>
-      <c r="H8" s="255"/>
-      <c r="I8" s="255"/>
-      <c r="J8" s="255"/>
-      <c r="K8" s="256"/>
+      <c r="B8" s="275"/>
+      <c r="C8" s="275"/>
+      <c r="D8" s="275"/>
+      <c r="E8" s="275"/>
+      <c r="F8" s="275"/>
+      <c r="G8" s="275"/>
+      <c r="H8" s="275"/>
+      <c r="I8" s="275"/>
+      <c r="J8" s="275"/>
+      <c r="K8" s="276"/>
     </row>
     <row r="9" spans="1:11" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="257"/>
-      <c r="B9" s="258"/>
-      <c r="C9" s="258"/>
-      <c r="D9" s="258"/>
-      <c r="E9" s="258"/>
-      <c r="F9" s="258"/>
-      <c r="G9" s="258"/>
-      <c r="H9" s="258"/>
-      <c r="I9" s="258"/>
-      <c r="J9" s="258"/>
-      <c r="K9" s="259"/>
+      <c r="A9" s="277"/>
+      <c r="B9" s="278"/>
+      <c r="C9" s="278"/>
+      <c r="D9" s="278"/>
+      <c r="E9" s="278"/>
+      <c r="F9" s="278"/>
+      <c r="G9" s="278"/>
+      <c r="H9" s="278"/>
+      <c r="I9" s="278"/>
+      <c r="J9" s="278"/>
+      <c r="K9" s="279"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="154"/>
@@ -5608,62 +5611,62 @@
       <c r="F10" s="140"/>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="270" t="s">
+      <c r="A11" s="253" t="s">
         <v>274</v>
       </c>
-      <c r="B11" s="271"/>
-      <c r="C11" s="271"/>
-      <c r="D11" s="272"/>
+      <c r="B11" s="254"/>
+      <c r="C11" s="254"/>
+      <c r="D11" s="255"/>
       <c r="E11" s="86"/>
       <c r="F11" s="140"/>
     </row>
     <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="273" t="s">
+      <c r="A12" s="256" t="s">
         <v>163</v>
       </c>
-      <c r="B12" s="274"/>
-      <c r="C12" s="275" t="s">
+      <c r="B12" s="257"/>
+      <c r="C12" s="258" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="276"/>
+      <c r="D12" s="259"/>
       <c r="E12" s="86"/>
       <c r="F12" s="140"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="277"/>
-      <c r="B13" s="278"/>
-      <c r="C13" s="279"/>
-      <c r="D13" s="280"/>
+      <c r="A13" s="260"/>
+      <c r="B13" s="261"/>
+      <c r="C13" s="262"/>
+      <c r="D13" s="263"/>
       <c r="E13" s="86"/>
       <c r="F13" s="140"/>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="270" t="s">
+      <c r="A15" s="253" t="s">
         <v>275</v>
       </c>
-      <c r="B15" s="272"/>
-      <c r="E15" s="270" t="s">
+      <c r="B15" s="255"/>
+      <c r="E15" s="253" t="s">
         <v>315</v>
       </c>
-      <c r="F15" s="271"/>
-      <c r="G15" s="271"/>
-      <c r="H15" s="271"/>
-      <c r="I15" s="272"/>
+      <c r="F15" s="254"/>
+      <c r="G15" s="254"/>
+      <c r="H15" s="254"/>
+      <c r="I15" s="255"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="265" t="s">
+      <c r="A16" s="264" t="s">
         <v>236</v>
       </c>
-      <c r="B16" s="266"/>
+      <c r="B16" s="265"/>
       <c r="D16" s="87"/>
-      <c r="E16" s="260" t="s">
+      <c r="E16" s="280" t="s">
         <v>197</v>
       </c>
-      <c r="F16" s="261"/>
-      <c r="G16" s="261"/>
-      <c r="H16" s="261"/>
-      <c r="I16" s="262"/>
+      <c r="F16" s="281"/>
+      <c r="G16" s="281"/>
+      <c r="H16" s="281"/>
+      <c r="I16" s="282"/>
     </row>
     <row r="17" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="155" t="s">
@@ -5673,10 +5676,10 @@
         <v>278</v>
       </c>
       <c r="C17" s="88"/>
-      <c r="E17" s="263" t="s">
+      <c r="E17" s="283" t="s">
         <v>235</v>
       </c>
-      <c r="F17" s="264"/>
+      <c r="F17" s="284"/>
       <c r="G17" s="199" t="s">
         <v>159</v>
       </c>
@@ -5706,7 +5709,7 @@
       <c r="H18" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="I18" s="239" t="s">
+      <c r="I18" s="268" t="s">
         <v>486</v>
       </c>
       <c r="J18" s="80"/>
@@ -5729,7 +5732,7 @@
       <c r="H19" s="73" t="s">
         <v>196</v>
       </c>
-      <c r="I19" s="239"/>
+      <c r="I19" s="268"/>
       <c r="J19" s="80"/>
     </row>
     <row r="20" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -5746,7 +5749,7 @@
       </c>
       <c r="G20" s="70"/>
       <c r="H20" s="70"/>
-      <c r="I20" s="240"/>
+      <c r="I20" s="269"/>
       <c r="J20" s="80"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -5768,24 +5771,24 @@
       <c r="A23" s="159"/>
       <c r="B23" s="91"/>
       <c r="C23" s="90"/>
-      <c r="E23" s="241" t="s">
+      <c r="E23" s="248" t="s">
         <v>198</v>
       </c>
-      <c r="F23" s="242"/>
-      <c r="G23" s="242"/>
-      <c r="H23" s="242"/>
-      <c r="I23" s="243"/>
+      <c r="F23" s="270"/>
+      <c r="G23" s="270"/>
+      <c r="H23" s="270"/>
+      <c r="I23" s="249"/>
     </row>
     <row r="24" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="241" t="s">
+      <c r="A24" s="248" t="s">
         <v>240</v>
       </c>
-      <c r="B24" s="243"/>
+      <c r="B24" s="249"/>
       <c r="C24" s="31"/>
-      <c r="E24" s="247" t="s">
+      <c r="E24" s="288" t="s">
         <v>235</v>
       </c>
-      <c r="F24" s="248"/>
+      <c r="F24" s="289"/>
       <c r="G24" s="199" t="s">
         <v>159</v>
       </c>
@@ -5814,7 +5817,7 @@
       <c r="H25" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="I25" s="244" t="s">
+      <c r="I25" s="285" t="s">
         <v>487</v>
       </c>
     </row>
@@ -5838,7 +5841,7 @@
       <c r="H26" s="73" t="s">
         <v>201</v>
       </c>
-      <c r="I26" s="245"/>
+      <c r="I26" s="286"/>
     </row>
     <row r="27" spans="1:10" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="157" t="s">
@@ -5854,7 +5857,7 @@
       </c>
       <c r="G27" s="70"/>
       <c r="H27" s="70"/>
-      <c r="I27" s="246"/>
+      <c r="I27" s="287"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="157" t="s">
@@ -5878,22 +5881,22 @@
       <c r="A30" s="158"/>
       <c r="B30" s="115"/>
       <c r="C30" s="88"/>
-      <c r="E30" s="241" t="s">
+      <c r="E30" s="248" t="s">
         <v>199</v>
       </c>
-      <c r="F30" s="242"/>
-      <c r="G30" s="242"/>
-      <c r="H30" s="242"/>
-      <c r="I30" s="243"/>
+      <c r="F30" s="270"/>
+      <c r="G30" s="270"/>
+      <c r="H30" s="270"/>
+      <c r="I30" s="249"/>
     </row>
     <row r="31" spans="1:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="159"/>
       <c r="B31" s="90"/>
       <c r="C31" s="90"/>
-      <c r="E31" s="249" t="s">
+      <c r="E31" s="290" t="s">
         <v>464</v>
       </c>
-      <c r="F31" s="250"/>
+      <c r="F31" s="291"/>
       <c r="G31" s="197" t="s">
         <v>159</v>
       </c>
@@ -5905,10 +5908,10 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="241" t="s">
+      <c r="A32" s="248" t="s">
         <v>241</v>
       </c>
-      <c r="B32" s="243"/>
+      <c r="B32" s="249"/>
       <c r="C32" s="31"/>
       <c r="E32" s="82">
         <v>1</v>
@@ -5918,7 +5921,7 @@
       </c>
       <c r="G32" s="32"/>
       <c r="H32" s="73"/>
-      <c r="I32" s="239"/>
+      <c r="I32" s="268"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="155" t="s">
@@ -5938,7 +5941,7 @@
         <v>5</v>
       </c>
       <c r="H33" s="32"/>
-      <c r="I33" s="239"/>
+      <c r="I33" s="268"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="156" t="s">
@@ -5953,7 +5956,7 @@
       <c r="F34" s="92"/>
       <c r="G34" s="32"/>
       <c r="H34" s="73"/>
-      <c r="I34" s="239"/>
+      <c r="I34" s="268"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="157" t="s">
@@ -5966,7 +5969,7 @@
       <c r="F35" s="92"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
-      <c r="I35" s="239"/>
+      <c r="I35" s="268"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="157" t="s">
@@ -5979,7 +5982,7 @@
       <c r="F36" s="92"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
-      <c r="I36" s="239"/>
+      <c r="I36" s="268"/>
     </row>
     <row r="37" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="157" t="s">
@@ -5992,7 +5995,7 @@
       <c r="F37" s="138"/>
       <c r="G37" s="70"/>
       <c r="H37" s="70"/>
-      <c r="I37" s="240"/>
+      <c r="I37" s="269"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="158" t="s">
@@ -6005,17 +6008,17 @@
       <c r="B39" s="119"/>
     </row>
     <row r="40" spans="1:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="E40" s="241" t="s">
+      <c r="E40" s="248" t="s">
         <v>200</v>
       </c>
-      <c r="F40" s="242"/>
-      <c r="G40" s="242"/>
-      <c r="H40" s="242"/>
-      <c r="I40" s="243"/>
+      <c r="F40" s="270"/>
+      <c r="G40" s="270"/>
+      <c r="H40" s="270"/>
+      <c r="I40" s="249"/>
     </row>
     <row r="41" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="E41" s="247"/>
-      <c r="F41" s="248"/>
+      <c r="E41" s="288"/>
+      <c r="F41" s="289"/>
       <c r="G41" s="81" t="s">
         <v>159</v>
       </c>
@@ -6033,7 +6036,7 @@
       <c r="F42" s="92"/>
       <c r="G42" s="32"/>
       <c r="H42" s="73"/>
-      <c r="I42" s="239"/>
+      <c r="I42" s="268"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E43" s="82">
@@ -6042,7 +6045,7 @@
       <c r="F43" s="92"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
-      <c r="I43" s="239"/>
+      <c r="I43" s="268"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E44" s="82">
@@ -6051,7 +6054,7 @@
       <c r="F44" s="92"/>
       <c r="G44" s="32"/>
       <c r="H44" s="73"/>
-      <c r="I44" s="239"/>
+      <c r="I44" s="268"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E45" s="82">
@@ -6060,7 +6063,7 @@
       <c r="F45" s="92"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
-      <c r="I45" s="239"/>
+      <c r="I45" s="268"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E46" s="82">
@@ -6069,7 +6072,7 @@
       <c r="F46" s="92"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
-      <c r="I46" s="239"/>
+      <c r="I46" s="268"/>
     </row>
     <row r="47" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E47" s="83">
@@ -6078,11 +6081,25 @@
       <c r="F47" s="138"/>
       <c r="G47" s="70"/>
       <c r="H47" s="70"/>
-      <c r="I47" s="240"/>
+      <c r="I47" s="269"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="I42:I47"/>
+    <mergeCell ref="E40:I40"/>
+    <mergeCell ref="I18:I20"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="E16:I16"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="A16:B16"/>
     <mergeCell ref="A24:B24"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A3:B3"/>
@@ -6098,20 +6115,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="I32:I37"/>
     <mergeCell ref="E30:I30"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="E16:I16"/>
-    <mergeCell ref="E23:I23"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="I42:I47"/>
-    <mergeCell ref="E40:I40"/>
-    <mergeCell ref="I18:I20"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6125,8 +6128,8 @@
   </sheetPr>
   <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A16" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6151,32 +6154,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="1" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="285" t="s">
+      <c r="A1" s="294" t="s">
         <v>379</v>
       </c>
-      <c r="B1" s="286"/>
-      <c r="C1" s="286"/>
-      <c r="D1" s="286"/>
-      <c r="E1" s="286"/>
-      <c r="F1" s="286"/>
-      <c r="G1" s="286"/>
-      <c r="H1" s="286"/>
-      <c r="I1" s="286"/>
-      <c r="J1" s="287"/>
+      <c r="B1" s="295"/>
+      <c r="C1" s="295"/>
+      <c r="D1" s="295"/>
+      <c r="E1" s="295"/>
+      <c r="F1" s="295"/>
+      <c r="G1" s="295"/>
+      <c r="H1" s="295"/>
+      <c r="I1" s="295"/>
+      <c r="J1" s="296"/>
     </row>
     <row r="2" spans="1:15" s="1" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="288" t="s">
+      <c r="A2" s="297" t="s">
         <v>242</v>
       </c>
-      <c r="B2" s="289"/>
-      <c r="C2" s="289"/>
-      <c r="D2" s="289"/>
-      <c r="E2" s="289"/>
-      <c r="F2" s="289"/>
-      <c r="G2" s="289"/>
-      <c r="H2" s="289"/>
-      <c r="I2" s="289"/>
-      <c r="J2" s="290"/>
+      <c r="B2" s="298"/>
+      <c r="C2" s="298"/>
+      <c r="D2" s="298"/>
+      <c r="E2" s="298"/>
+      <c r="F2" s="298"/>
+      <c r="G2" s="298"/>
+      <c r="H2" s="298"/>
+      <c r="I2" s="298"/>
+      <c r="J2" s="299"/>
       <c r="K2" s="78"/>
       <c r="L2" s="78"/>
       <c r="M2" s="74"/>
@@ -6190,13 +6193,13 @@
       <c r="B3" s="175" t="s">
         <v>317</v>
       </c>
-      <c r="C3" s="291" t="s">
+      <c r="C3" s="300" t="s">
         <v>290</v>
       </c>
-      <c r="D3" s="292"/>
-      <c r="E3" s="292"/>
-      <c r="F3" s="292"/>
-      <c r="G3" s="293"/>
+      <c r="D3" s="301"/>
+      <c r="E3" s="301"/>
+      <c r="F3" s="301"/>
+      <c r="G3" s="302"/>
       <c r="H3" s="175" t="s">
         <v>318</v>
       </c>
@@ -6887,26 +6890,26 @@
     </row>
     <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:18" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="353" t="s">
+      <c r="A28" s="312" t="s">
         <v>243</v>
       </c>
-      <c r="B28" s="354"/>
-      <c r="C28" s="354"/>
-      <c r="D28" s="354"/>
-      <c r="E28" s="354"/>
-      <c r="F28" s="354"/>
-      <c r="G28" s="354"/>
-      <c r="H28" s="354"/>
-      <c r="I28" s="354"/>
-      <c r="J28" s="354"/>
-      <c r="K28" s="354"/>
-      <c r="L28" s="354"/>
-      <c r="M28" s="354"/>
-      <c r="N28" s="354"/>
-      <c r="O28" s="354"/>
-      <c r="P28" s="354"/>
-      <c r="Q28" s="354"/>
-      <c r="R28" s="354"/>
+      <c r="B28" s="313"/>
+      <c r="C28" s="313"/>
+      <c r="D28" s="313"/>
+      <c r="E28" s="313"/>
+      <c r="F28" s="313"/>
+      <c r="G28" s="313"/>
+      <c r="H28" s="313"/>
+      <c r="I28" s="313"/>
+      <c r="J28" s="313"/>
+      <c r="K28" s="313"/>
+      <c r="L28" s="313"/>
+      <c r="M28" s="313"/>
+      <c r="N28" s="313"/>
+      <c r="O28" s="313"/>
+      <c r="P28" s="313"/>
+      <c r="Q28" s="313"/>
+      <c r="R28" s="313"/>
     </row>
     <row r="29" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="135" t="s">
@@ -6945,7 +6948,7 @@
       <c r="L29" s="121" t="s">
         <v>270</v>
       </c>
-      <c r="M29" s="351" t="s">
+      <c r="M29" s="239" t="s">
         <v>270</v>
       </c>
       <c r="N29" s="121" t="s">
@@ -6999,7 +7002,7 @@
       <c r="L30" s="95" t="s">
         <v>94</v>
       </c>
-      <c r="M30" s="352" t="s">
+      <c r="M30" s="240" t="s">
         <v>513</v>
       </c>
       <c r="N30" s="95" t="s">
@@ -7060,70 +7063,70 @@
     </row>
     <row r="32" spans="1:18" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:8" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A33" s="300" t="s">
+      <c r="A33" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B33" s="301"/>
-      <c r="C33" s="301"/>
-      <c r="D33" s="301"/>
-      <c r="E33" s="301"/>
-      <c r="F33" s="301"/>
-      <c r="G33" s="301"/>
-      <c r="H33" s="302"/>
+      <c r="B33" s="310"/>
+      <c r="C33" s="310"/>
+      <c r="D33" s="310"/>
+      <c r="E33" s="310"/>
+      <c r="F33" s="310"/>
+      <c r="G33" s="310"/>
+      <c r="H33" s="311"/>
     </row>
     <row r="34" spans="1:8" s="1" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="294" t="s">
+      <c r="A34" s="303" t="s">
         <v>361</v>
       </c>
-      <c r="B34" s="295"/>
-      <c r="C34" s="295"/>
-      <c r="D34" s="295"/>
-      <c r="E34" s="295"/>
-      <c r="F34" s="295"/>
-      <c r="G34" s="295"/>
-      <c r="H34" s="296"/>
+      <c r="B34" s="304"/>
+      <c r="C34" s="304"/>
+      <c r="D34" s="304"/>
+      <c r="E34" s="304"/>
+      <c r="F34" s="304"/>
+      <c r="G34" s="304"/>
+      <c r="H34" s="305"/>
     </row>
     <row r="35" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="294"/>
-      <c r="B35" s="295"/>
-      <c r="C35" s="295"/>
-      <c r="D35" s="295"/>
-      <c r="E35" s="295"/>
-      <c r="F35" s="295"/>
-      <c r="G35" s="295"/>
-      <c r="H35" s="296"/>
+      <c r="A35" s="303"/>
+      <c r="B35" s="304"/>
+      <c r="C35" s="304"/>
+      <c r="D35" s="304"/>
+      <c r="E35" s="304"/>
+      <c r="F35" s="304"/>
+      <c r="G35" s="304"/>
+      <c r="H35" s="305"/>
     </row>
     <row r="36" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="294"/>
-      <c r="B36" s="295"/>
-      <c r="C36" s="295"/>
-      <c r="D36" s="295"/>
-      <c r="E36" s="295"/>
-      <c r="F36" s="295"/>
-      <c r="G36" s="295"/>
-      <c r="H36" s="296"/>
+      <c r="A36" s="303"/>
+      <c r="B36" s="304"/>
+      <c r="C36" s="304"/>
+      <c r="D36" s="304"/>
+      <c r="E36" s="304"/>
+      <c r="F36" s="304"/>
+      <c r="G36" s="304"/>
+      <c r="H36" s="305"/>
     </row>
     <row r="37" spans="1:8" s="1" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="297"/>
-      <c r="B37" s="298"/>
-      <c r="C37" s="298"/>
-      <c r="D37" s="298"/>
-      <c r="E37" s="298"/>
-      <c r="F37" s="298"/>
-      <c r="G37" s="298"/>
-      <c r="H37" s="299"/>
+      <c r="A37" s="306"/>
+      <c r="B37" s="307"/>
+      <c r="C37" s="307"/>
+      <c r="D37" s="307"/>
+      <c r="E37" s="307"/>
+      <c r="F37" s="307"/>
+      <c r="G37" s="307"/>
+      <c r="H37" s="308"/>
     </row>
     <row r="38" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="39" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="284" t="s">
+      <c r="A39" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B39" s="284"/>
-      <c r="C39" s="284"/>
-      <c r="D39" s="284"/>
-      <c r="E39" s="284"/>
-      <c r="F39" s="284"/>
-      <c r="G39" s="284"/>
+      <c r="B39" s="293"/>
+      <c r="C39" s="293"/>
+      <c r="D39" s="293"/>
+      <c r="E39" s="293"/>
+      <c r="F39" s="293"/>
+      <c r="G39" s="293"/>
     </row>
     <row r="40" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="77" t="s">
@@ -7135,12 +7138,12 @@
       <c r="C40" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D40" s="283" t="s">
+      <c r="D40" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E40" s="283"/>
-      <c r="F40" s="283"/>
-      <c r="G40" s="283"/>
+      <c r="E40" s="292"/>
+      <c r="F40" s="292"/>
+      <c r="G40" s="292"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -7685,32 +7688,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="306" t="s">
+      <c r="A1" s="317" t="s">
         <v>380</v>
       </c>
-      <c r="B1" s="307"/>
-      <c r="C1" s="307"/>
-      <c r="D1" s="307"/>
-      <c r="E1" s="307"/>
-      <c r="F1" s="307"/>
-      <c r="G1" s="307"/>
-      <c r="H1" s="307"/>
-      <c r="I1" s="307"/>
-      <c r="J1" s="308"/>
+      <c r="B1" s="318"/>
+      <c r="C1" s="318"/>
+      <c r="D1" s="318"/>
+      <c r="E1" s="318"/>
+      <c r="F1" s="318"/>
+      <c r="G1" s="318"/>
+      <c r="H1" s="318"/>
+      <c r="I1" s="318"/>
+      <c r="J1" s="319"/>
     </row>
     <row r="2" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="303" t="s">
+      <c r="A2" s="314" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="304"/>
-      <c r="C2" s="304"/>
-      <c r="D2" s="304"/>
-      <c r="E2" s="304"/>
-      <c r="F2" s="304"/>
-      <c r="G2" s="304"/>
-      <c r="H2" s="304"/>
-      <c r="I2" s="304"/>
-      <c r="J2" s="305"/>
+      <c r="B2" s="315"/>
+      <c r="C2" s="315"/>
+      <c r="D2" s="315"/>
+      <c r="E2" s="315"/>
+      <c r="F2" s="315"/>
+      <c r="G2" s="315"/>
+      <c r="H2" s="315"/>
+      <c r="I2" s="315"/>
+      <c r="J2" s="316"/>
     </row>
     <row r="3" spans="1:10" s="111" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="129" t="s">
@@ -7789,18 +7792,18 @@
       <c r="J5" s="163"/>
     </row>
     <row r="6" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="303" t="s">
+      <c r="A6" s="314" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="304"/>
-      <c r="C6" s="304"/>
-      <c r="D6" s="304"/>
-      <c r="E6" s="304"/>
-      <c r="F6" s="304"/>
-      <c r="G6" s="304"/>
-      <c r="H6" s="304"/>
-      <c r="I6" s="304"/>
-      <c r="J6" s="305"/>
+      <c r="B6" s="315"/>
+      <c r="C6" s="315"/>
+      <c r="D6" s="315"/>
+      <c r="E6" s="315"/>
+      <c r="F6" s="315"/>
+      <c r="G6" s="315"/>
+      <c r="H6" s="315"/>
+      <c r="I6" s="315"/>
+      <c r="J6" s="316"/>
     </row>
     <row r="7" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="122" t="s">
@@ -7851,18 +7854,18 @@
       <c r="J9" s="71"/>
     </row>
     <row r="10" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="303" t="s">
+      <c r="A10" s="314" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="304"/>
-      <c r="C10" s="304"/>
-      <c r="D10" s="304"/>
-      <c r="E10" s="304"/>
-      <c r="F10" s="304"/>
-      <c r="G10" s="304"/>
-      <c r="H10" s="304"/>
-      <c r="I10" s="304"/>
-      <c r="J10" s="305"/>
+      <c r="B10" s="315"/>
+      <c r="C10" s="315"/>
+      <c r="D10" s="315"/>
+      <c r="E10" s="315"/>
+      <c r="F10" s="315"/>
+      <c r="G10" s="315"/>
+      <c r="H10" s="315"/>
+      <c r="I10" s="315"/>
+      <c r="J10" s="316"/>
     </row>
     <row r="11" spans="1:10" s="111" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="125"/>
@@ -8017,18 +8020,18 @@
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="309" t="s">
+      <c r="A17" s="320" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="310"/>
-      <c r="C17" s="310"/>
-      <c r="D17" s="310"/>
-      <c r="E17" s="310"/>
-      <c r="F17" s="310"/>
-      <c r="G17" s="310"/>
-      <c r="H17" s="310"/>
-      <c r="I17" s="310"/>
-      <c r="J17" s="311"/>
+      <c r="B17" s="321"/>
+      <c r="C17" s="321"/>
+      <c r="D17" s="321"/>
+      <c r="E17" s="321"/>
+      <c r="F17" s="321"/>
+      <c r="G17" s="321"/>
+      <c r="H17" s="321"/>
+      <c r="I17" s="321"/>
+      <c r="J17" s="322"/>
     </row>
     <row r="18" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="209"/>
@@ -8113,18 +8116,18 @@
       <c r="J21" s="223"/>
     </row>
     <row r="22" spans="1:10" s="111" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="303" t="s">
+      <c r="A22" s="314" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="304"/>
-      <c r="C22" s="304"/>
-      <c r="D22" s="304"/>
-      <c r="E22" s="304"/>
-      <c r="F22" s="304"/>
-      <c r="G22" s="304"/>
-      <c r="H22" s="304"/>
-      <c r="I22" s="304"/>
-      <c r="J22" s="305"/>
+      <c r="B22" s="315"/>
+      <c r="C22" s="315"/>
+      <c r="D22" s="315"/>
+      <c r="E22" s="315"/>
+      <c r="F22" s="315"/>
+      <c r="G22" s="315"/>
+      <c r="H22" s="315"/>
+      <c r="I22" s="315"/>
+      <c r="J22" s="316"/>
     </row>
     <row r="23" spans="1:10" s="111" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="129" t="s">
@@ -8187,18 +8190,18 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="309" t="s">
+      <c r="A26" s="320" t="s">
         <v>507</v>
       </c>
-      <c r="B26" s="310"/>
-      <c r="C26" s="310"/>
-      <c r="D26" s="310"/>
-      <c r="E26" s="310"/>
-      <c r="F26" s="310"/>
-      <c r="G26" s="310"/>
-      <c r="H26" s="310"/>
-      <c r="I26" s="310"/>
-      <c r="J26" s="311"/>
+      <c r="B26" s="321"/>
+      <c r="C26" s="321"/>
+      <c r="D26" s="321"/>
+      <c r="E26" s="321"/>
+      <c r="F26" s="321"/>
+      <c r="G26" s="321"/>
+      <c r="H26" s="321"/>
+      <c r="I26" s="321"/>
+      <c r="J26" s="322"/>
     </row>
     <row r="27" spans="1:10" s="111" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="224" t="s">
@@ -8273,18 +8276,18 @@
       <c r="J29" s="238"/>
     </row>
     <row r="30" spans="1:10" s="111" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="303" t="s">
+      <c r="A30" s="314" t="s">
         <v>153</v>
       </c>
-      <c r="B30" s="304"/>
-      <c r="C30" s="304"/>
-      <c r="D30" s="304"/>
-      <c r="E30" s="304"/>
-      <c r="F30" s="304"/>
-      <c r="G30" s="304"/>
-      <c r="H30" s="304"/>
-      <c r="I30" s="304"/>
-      <c r="J30" s="305"/>
+      <c r="B30" s="315"/>
+      <c r="C30" s="315"/>
+      <c r="D30" s="315"/>
+      <c r="E30" s="315"/>
+      <c r="F30" s="315"/>
+      <c r="G30" s="315"/>
+      <c r="H30" s="315"/>
+      <c r="I30" s="315"/>
+      <c r="J30" s="316"/>
     </row>
     <row r="31" spans="1:10" s="111" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="129" t="s">
@@ -8346,58 +8349,58 @@
     </row>
     <row r="34" spans="1:10" s="111" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:10" s="111" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="300" t="s">
+      <c r="A35" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B35" s="301"/>
-      <c r="C35" s="301"/>
-      <c r="D35" s="301"/>
-      <c r="E35" s="301"/>
-      <c r="F35" s="301"/>
-      <c r="G35" s="301"/>
-      <c r="H35" s="302"/>
+      <c r="B35" s="310"/>
+      <c r="C35" s="310"/>
+      <c r="D35" s="310"/>
+      <c r="E35" s="310"/>
+      <c r="F35" s="310"/>
+      <c r="G35" s="310"/>
+      <c r="H35" s="311"/>
     </row>
     <row r="36" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="294" t="s">
+      <c r="A36" s="303" t="s">
         <v>360</v>
       </c>
-      <c r="B36" s="295"/>
-      <c r="C36" s="295"/>
-      <c r="D36" s="295"/>
-      <c r="E36" s="295"/>
-      <c r="F36" s="295"/>
-      <c r="G36" s="295"/>
-      <c r="H36" s="296"/>
+      <c r="B36" s="304"/>
+      <c r="C36" s="304"/>
+      <c r="D36" s="304"/>
+      <c r="E36" s="304"/>
+      <c r="F36" s="304"/>
+      <c r="G36" s="304"/>
+      <c r="H36" s="305"/>
     </row>
     <row r="37" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="294"/>
-      <c r="B37" s="295"/>
-      <c r="C37" s="295"/>
-      <c r="D37" s="295"/>
-      <c r="E37" s="295"/>
-      <c r="F37" s="295"/>
-      <c r="G37" s="295"/>
-      <c r="H37" s="296"/>
+      <c r="A37" s="303"/>
+      <c r="B37" s="304"/>
+      <c r="C37" s="304"/>
+      <c r="D37" s="304"/>
+      <c r="E37" s="304"/>
+      <c r="F37" s="304"/>
+      <c r="G37" s="304"/>
+      <c r="H37" s="305"/>
     </row>
     <row r="38" spans="1:10" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="294"/>
-      <c r="B38" s="295"/>
-      <c r="C38" s="295"/>
-      <c r="D38" s="295"/>
-      <c r="E38" s="295"/>
-      <c r="F38" s="295"/>
-      <c r="G38" s="295"/>
-      <c r="H38" s="296"/>
+      <c r="A38" s="303"/>
+      <c r="B38" s="304"/>
+      <c r="C38" s="304"/>
+      <c r="D38" s="304"/>
+      <c r="E38" s="304"/>
+      <c r="F38" s="304"/>
+      <c r="G38" s="304"/>
+      <c r="H38" s="305"/>
     </row>
     <row r="39" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="297"/>
-      <c r="B39" s="298"/>
-      <c r="C39" s="298"/>
-      <c r="D39" s="298"/>
-      <c r="E39" s="298"/>
-      <c r="F39" s="298"/>
-      <c r="G39" s="298"/>
-      <c r="H39" s="299"/>
+      <c r="A39" s="306"/>
+      <c r="B39" s="307"/>
+      <c r="C39" s="307"/>
+      <c r="D39" s="307"/>
+      <c r="E39" s="307"/>
+      <c r="F39" s="307"/>
+      <c r="G39" s="307"/>
+      <c r="H39" s="308"/>
       <c r="I39" s="111"/>
       <c r="J39" s="111"/>
     </row>
@@ -8414,15 +8417,15 @@
       <c r="J40" s="111"/>
     </row>
     <row r="41" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A41" s="284" t="s">
+      <c r="A41" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B41" s="284"/>
-      <c r="C41" s="284"/>
-      <c r="D41" s="284"/>
-      <c r="E41" s="284"/>
-      <c r="F41" s="284"/>
-      <c r="G41" s="284"/>
+      <c r="B41" s="293"/>
+      <c r="C41" s="293"/>
+      <c r="D41" s="293"/>
+      <c r="E41" s="293"/>
+      <c r="F41" s="293"/>
+      <c r="G41" s="293"/>
       <c r="H41" s="111"/>
       <c r="I41" s="111"/>
       <c r="J41" s="111"/>
@@ -8437,12 +8440,12 @@
       <c r="C42" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D42" s="283" t="s">
+      <c r="D42" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E42" s="283"/>
-      <c r="F42" s="283"/>
-      <c r="G42" s="283"/>
+      <c r="E42" s="292"/>
+      <c r="F42" s="292"/>
+      <c r="G42" s="292"/>
       <c r="H42" s="111"/>
       <c r="I42" s="111"/>
       <c r="J42" s="111"/>
@@ -8684,68 +8687,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="327" t="s">
         <v>244</v>
       </c>
-      <c r="B1" s="323"/>
-      <c r="C1" s="323"/>
-      <c r="D1" s="323"/>
-      <c r="E1" s="323"/>
-      <c r="F1" s="323"/>
-      <c r="G1" s="323"/>
-      <c r="H1" s="323"/>
-      <c r="I1" s="323"/>
-      <c r="J1" s="323"/>
-      <c r="K1" s="323"/>
-      <c r="L1" s="323"/>
-      <c r="M1" s="323"/>
-      <c r="N1" s="323"/>
-      <c r="O1" s="323"/>
+      <c r="B1" s="327"/>
+      <c r="C1" s="327"/>
+      <c r="D1" s="327"/>
+      <c r="E1" s="327"/>
+      <c r="F1" s="327"/>
+      <c r="G1" s="327"/>
+      <c r="H1" s="327"/>
+      <c r="I1" s="327"/>
+      <c r="J1" s="327"/>
+      <c r="K1" s="327"/>
+      <c r="L1" s="327"/>
+      <c r="M1" s="327"/>
+      <c r="N1" s="327"/>
+      <c r="O1" s="327"/>
       <c r="P1" s="30"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="317" t="s">
+      <c r="A2" s="338" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="318"/>
-      <c r="C2" s="318"/>
-      <c r="D2" s="318"/>
-      <c r="E2" s="318"/>
-      <c r="F2" s="319"/>
-      <c r="G2" s="324" t="s">
+      <c r="B2" s="339"/>
+      <c r="C2" s="339"/>
+      <c r="D2" s="339"/>
+      <c r="E2" s="339"/>
+      <c r="F2" s="340"/>
+      <c r="G2" s="328" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="324"/>
-      <c r="I2" s="324"/>
-      <c r="J2" s="324"/>
-      <c r="K2" s="324"/>
-      <c r="L2" s="324"/>
-      <c r="M2" s="313" t="s">
+      <c r="H2" s="328"/>
+      <c r="I2" s="328"/>
+      <c r="J2" s="328"/>
+      <c r="K2" s="328"/>
+      <c r="L2" s="328"/>
+      <c r="M2" s="334" t="s">
         <v>295</v>
       </c>
-      <c r="N2" s="313"/>
-      <c r="O2" s="313"/>
+      <c r="N2" s="334"/>
+      <c r="O2" s="334"/>
       <c r="P2" s="87"/>
       <c r="Q2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="320" t="s">
+      <c r="A3" s="341" t="s">
         <v>493</v>
       </c>
-      <c r="B3" s="321"/>
-      <c r="C3" s="321"/>
-      <c r="D3" s="321"/>
-      <c r="E3" s="321"/>
-      <c r="F3" s="322"/>
-      <c r="G3" s="326" t="s">
+      <c r="B3" s="342"/>
+      <c r="C3" s="342"/>
+      <c r="D3" s="342"/>
+      <c r="E3" s="342"/>
+      <c r="F3" s="343"/>
+      <c r="G3" s="330" t="s">
         <v>301</v>
       </c>
-      <c r="H3" s="326"/>
-      <c r="I3" s="326"/>
-      <c r="J3" s="326"/>
-      <c r="K3" s="326"/>
-      <c r="L3" s="326"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="330"/>
+      <c r="J3" s="330"/>
+      <c r="K3" s="330"/>
+      <c r="L3" s="330"/>
       <c r="M3" s="203" t="s">
         <v>299</v>
       </c>
@@ -8758,24 +8761,24 @@
       <c r="P3" s="193"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="327" t="s">
+      <c r="A4" s="331" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="328"/>
-      <c r="C4" s="328"/>
-      <c r="D4" s="328"/>
-      <c r="E4" s="328"/>
-      <c r="F4" s="329"/>
-      <c r="G4" s="325" t="s">
+      <c r="B4" s="332"/>
+      <c r="C4" s="332"/>
+      <c r="D4" s="332"/>
+      <c r="E4" s="332"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="329" t="s">
         <v>247</v>
       </c>
-      <c r="H4" s="325"/>
-      <c r="I4" s="325"/>
-      <c r="J4" s="325" t="s">
+      <c r="H4" s="329"/>
+      <c r="I4" s="329"/>
+      <c r="J4" s="329" t="s">
         <v>302</v>
       </c>
-      <c r="K4" s="325"/>
-      <c r="L4" s="325"/>
+      <c r="K4" s="329"/>
+      <c r="L4" s="329"/>
       <c r="M4" s="204" t="s">
         <v>154</v>
       </c>
@@ -8787,22 +8790,22 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="330"/>
-      <c r="B5" s="331"/>
-      <c r="C5" s="331"/>
-      <c r="D5" s="331"/>
-      <c r="E5" s="331"/>
-      <c r="F5" s="332"/>
-      <c r="G5" s="312" t="s">
+      <c r="A5" s="324"/>
+      <c r="B5" s="325"/>
+      <c r="C5" s="325"/>
+      <c r="D5" s="325"/>
+      <c r="E5" s="325"/>
+      <c r="F5" s="326"/>
+      <c r="G5" s="323" t="s">
         <v>278</v>
       </c>
-      <c r="H5" s="312"/>
-      <c r="I5" s="312"/>
-      <c r="J5" s="312" t="s">
+      <c r="H5" s="323"/>
+      <c r="I5" s="323"/>
+      <c r="J5" s="323" t="s">
         <v>292</v>
       </c>
-      <c r="K5" s="312"/>
-      <c r="L5" s="312"/>
+      <c r="K5" s="323"/>
+      <c r="L5" s="323"/>
       <c r="M5" s="205"/>
       <c r="N5" s="205" t="s">
         <v>384</v>
@@ -8812,22 +8815,22 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="330" t="s">
+      <c r="A6" s="324" t="s">
         <v>495</v>
       </c>
-      <c r="B6" s="331"/>
-      <c r="C6" s="331"/>
-      <c r="D6" s="331"/>
-      <c r="E6" s="331"/>
-      <c r="F6" s="332"/>
-      <c r="G6" s="312" t="s">
+      <c r="B6" s="325"/>
+      <c r="C6" s="325"/>
+      <c r="D6" s="325"/>
+      <c r="E6" s="325"/>
+      <c r="F6" s="326"/>
+      <c r="G6" s="323" t="s">
         <v>285</v>
       </c>
-      <c r="H6" s="312"/>
-      <c r="I6" s="312"/>
-      <c r="J6" s="312"/>
-      <c r="K6" s="312"/>
-      <c r="L6" s="312"/>
+      <c r="H6" s="323"/>
+      <c r="I6" s="323"/>
+      <c r="J6" s="323"/>
+      <c r="K6" s="323"/>
+      <c r="L6" s="323"/>
       <c r="M6" s="205"/>
       <c r="N6" s="205" t="s">
         <v>385</v>
@@ -8837,54 +8840,54 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="330" t="s">
+      <c r="A7" s="324" t="s">
         <v>496</v>
       </c>
-      <c r="B7" s="331"/>
-      <c r="C7" s="331"/>
-      <c r="D7" s="331"/>
-      <c r="E7" s="331"/>
-      <c r="F7" s="332"/>
-      <c r="G7" s="312"/>
-      <c r="H7" s="312"/>
-      <c r="I7" s="312"/>
-      <c r="J7" s="312"/>
-      <c r="K7" s="312"/>
-      <c r="L7" s="312"/>
+      <c r="B7" s="325"/>
+      <c r="C7" s="325"/>
+      <c r="D7" s="325"/>
+      <c r="E7" s="325"/>
+      <c r="F7" s="326"/>
+      <c r="G7" s="323"/>
+      <c r="H7" s="323"/>
+      <c r="I7" s="323"/>
+      <c r="J7" s="323"/>
+      <c r="K7" s="323"/>
+      <c r="L7" s="323"/>
       <c r="M7" s="205"/>
       <c r="N7" s="205"/>
       <c r="O7" s="206"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="330"/>
-      <c r="B8" s="331"/>
-      <c r="C8" s="331"/>
-      <c r="D8" s="331"/>
-      <c r="E8" s="331"/>
-      <c r="F8" s="332"/>
-      <c r="G8" s="312"/>
-      <c r="H8" s="312"/>
-      <c r="I8" s="312"/>
-      <c r="J8" s="312"/>
-      <c r="K8" s="312"/>
-      <c r="L8" s="312"/>
+      <c r="A8" s="324"/>
+      <c r="B8" s="325"/>
+      <c r="C8" s="325"/>
+      <c r="D8" s="325"/>
+      <c r="E8" s="325"/>
+      <c r="F8" s="326"/>
+      <c r="G8" s="323"/>
+      <c r="H8" s="323"/>
+      <c r="I8" s="323"/>
+      <c r="J8" s="323"/>
+      <c r="K8" s="323"/>
+      <c r="L8" s="323"/>
       <c r="M8" s="205"/>
       <c r="N8" s="205"/>
       <c r="O8" s="206"/>
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="314" t="s">
+      <c r="A10" s="335" t="s">
         <v>354</v>
       </c>
-      <c r="B10" s="315"/>
-      <c r="C10" s="315"/>
-      <c r="D10" s="315"/>
-      <c r="E10" s="315"/>
-      <c r="F10" s="315"/>
-      <c r="G10" s="315"/>
-      <c r="H10" s="315"/>
-      <c r="I10" s="316"/>
+      <c r="B10" s="336"/>
+      <c r="C10" s="336"/>
+      <c r="D10" s="336"/>
+      <c r="E10" s="336"/>
+      <c r="F10" s="336"/>
+      <c r="G10" s="336"/>
+      <c r="H10" s="336"/>
+      <c r="I10" s="337"/>
     </row>
     <row r="11" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
@@ -8899,7 +8902,7 @@
       <c r="D11" s="123" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="351" t="s">
+      <c r="E11" s="239" t="s">
         <v>270</v>
       </c>
       <c r="F11" s="123" t="s">
@@ -8931,7 +8934,7 @@
       <c r="D12" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="352" t="s">
+      <c r="E12" s="240" t="s">
         <v>513</v>
       </c>
       <c r="F12" s="145" t="s">
@@ -8974,69 +8977,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="300" t="s">
+      <c r="A15" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="301"/>
-      <c r="C15" s="301"/>
-      <c r="D15" s="301"/>
-      <c r="E15" s="301"/>
-      <c r="F15" s="301"/>
-      <c r="G15" s="301"/>
-      <c r="H15" s="302"/>
+      <c r="B15" s="310"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="310"/>
+      <c r="E15" s="310"/>
+      <c r="F15" s="310"/>
+      <c r="G15" s="310"/>
+      <c r="H15" s="311"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="294" t="s">
+      <c r="A16" s="303" t="s">
         <v>362</v>
       </c>
-      <c r="B16" s="295"/>
-      <c r="C16" s="295"/>
-      <c r="D16" s="295"/>
-      <c r="E16" s="295"/>
-      <c r="F16" s="295"/>
-      <c r="G16" s="295"/>
-      <c r="H16" s="296"/>
+      <c r="B16" s="304"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="304"/>
+      <c r="E16" s="304"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
+      <c r="H16" s="305"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="294"/>
-      <c r="B17" s="295"/>
-      <c r="C17" s="295"/>
-      <c r="D17" s="295"/>
-      <c r="E17" s="295"/>
-      <c r="F17" s="295"/>
-      <c r="G17" s="295"/>
-      <c r="H17" s="296"/>
+      <c r="A17" s="303"/>
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="304"/>
+      <c r="E17" s="304"/>
+      <c r="F17" s="304"/>
+      <c r="G17" s="304"/>
+      <c r="H17" s="305"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="294"/>
-      <c r="B18" s="295"/>
-      <c r="C18" s="295"/>
-      <c r="D18" s="295"/>
-      <c r="E18" s="295"/>
-      <c r="F18" s="295"/>
-      <c r="G18" s="295"/>
-      <c r="H18" s="296"/>
+      <c r="A18" s="303"/>
+      <c r="B18" s="304"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="304"/>
+      <c r="E18" s="304"/>
+      <c r="F18" s="304"/>
+      <c r="G18" s="304"/>
+      <c r="H18" s="305"/>
     </row>
     <row r="19" spans="1:8" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="297"/>
-      <c r="B19" s="298"/>
-      <c r="C19" s="298"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="298"/>
-      <c r="G19" s="298"/>
-      <c r="H19" s="299"/>
+      <c r="A19" s="306"/>
+      <c r="B19" s="307"/>
+      <c r="C19" s="307"/>
+      <c r="D19" s="307"/>
+      <c r="E19" s="307"/>
+      <c r="F19" s="307"/>
+      <c r="G19" s="307"/>
+      <c r="H19" s="308"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="284" t="s">
+      <c r="A21" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="284"/>
-      <c r="C21" s="284"/>
-      <c r="D21" s="284"/>
-      <c r="E21" s="284"/>
-      <c r="F21" s="284"/>
-      <c r="G21" s="284"/>
+      <c r="B21" s="293"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="293"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -9048,12 +9051,12 @@
       <c r="C22" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="283" t="s">
+      <c r="D22" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="283"/>
-      <c r="F22" s="283"/>
-      <c r="G22" s="283"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -9491,12 +9494,14 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D22:G22"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="A16:H19"/>
+    <mergeCell ref="A10:I10"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="G6:I6"/>
     <mergeCell ref="J6:L6"/>
@@ -9509,14 +9514,12 @@
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="M2:O2"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="A16:H19"/>
-    <mergeCell ref="A10:I10"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="D22:G22"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9608,68 +9611,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="323" t="s">
+      <c r="A1" s="327" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="323"/>
-      <c r="C1" s="323"/>
-      <c r="D1" s="323"/>
-      <c r="E1" s="323"/>
-      <c r="F1" s="323"/>
-      <c r="G1" s="323"/>
-      <c r="H1" s="323"/>
-      <c r="I1" s="323"/>
-      <c r="J1" s="323"/>
-      <c r="K1" s="323"/>
-      <c r="L1" s="323"/>
-      <c r="M1" s="323"/>
-      <c r="N1" s="323"/>
-      <c r="O1" s="323"/>
-      <c r="P1" s="323"/>
+      <c r="B1" s="327"/>
+      <c r="C1" s="327"/>
+      <c r="D1" s="327"/>
+      <c r="E1" s="327"/>
+      <c r="F1" s="327"/>
+      <c r="G1" s="327"/>
+      <c r="H1" s="327"/>
+      <c r="I1" s="327"/>
+      <c r="J1" s="327"/>
+      <c r="K1" s="327"/>
+      <c r="L1" s="327"/>
+      <c r="M1" s="327"/>
+      <c r="N1" s="327"/>
+      <c r="O1" s="327"/>
+      <c r="P1" s="327"/>
       <c r="Q1" s="30"/>
     </row>
     <row r="2" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="324" t="s">
+      <c r="A2" s="328" t="s">
         <v>279</v>
       </c>
-      <c r="B2" s="324"/>
-      <c r="C2" s="324"/>
-      <c r="D2" s="324"/>
-      <c r="E2" s="324"/>
-      <c r="F2" s="324"/>
-      <c r="G2" s="324" t="s">
+      <c r="B2" s="328"/>
+      <c r="C2" s="328"/>
+      <c r="D2" s="328"/>
+      <c r="E2" s="328"/>
+      <c r="F2" s="328"/>
+      <c r="G2" s="328" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="324"/>
-      <c r="I2" s="324"/>
-      <c r="J2" s="324"/>
-      <c r="K2" s="324"/>
-      <c r="L2" s="324"/>
-      <c r="M2" s="313" t="s">
+      <c r="H2" s="328"/>
+      <c r="I2" s="328"/>
+      <c r="J2" s="328"/>
+      <c r="K2" s="328"/>
+      <c r="L2" s="328"/>
+      <c r="M2" s="334" t="s">
         <v>294</v>
       </c>
-      <c r="N2" s="313"/>
-      <c r="O2" s="313"/>
-      <c r="P2" s="313"/>
+      <c r="N2" s="334"/>
+      <c r="O2" s="334"/>
+      <c r="P2" s="334"/>
       <c r="Q2" s="87"/>
     </row>
     <row r="3" spans="1:17" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="326" t="s">
+      <c r="A3" s="330" t="s">
         <v>497</v>
       </c>
-      <c r="B3" s="326"/>
-      <c r="C3" s="326"/>
-      <c r="D3" s="326"/>
-      <c r="E3" s="326"/>
-      <c r="F3" s="326"/>
-      <c r="G3" s="326" t="s">
+      <c r="B3" s="330"/>
+      <c r="C3" s="330"/>
+      <c r="D3" s="330"/>
+      <c r="E3" s="330"/>
+      <c r="F3" s="330"/>
+      <c r="G3" s="330" t="s">
         <v>296</v>
       </c>
-      <c r="H3" s="326"/>
-      <c r="I3" s="326"/>
-      <c r="J3" s="326"/>
-      <c r="K3" s="326"/>
-      <c r="L3" s="326"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="330"/>
+      <c r="J3" s="330"/>
+      <c r="K3" s="330"/>
+      <c r="L3" s="330"/>
       <c r="M3" s="203" t="s">
         <v>298</v>
       </c>
@@ -9685,22 +9688,22 @@
       <c r="Q3" s="192"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="327" t="s">
+      <c r="A4" s="331" t="s">
         <v>494</v>
       </c>
-      <c r="B4" s="328"/>
-      <c r="C4" s="328"/>
-      <c r="D4" s="328"/>
-      <c r="E4" s="328"/>
-      <c r="F4" s="329"/>
-      <c r="G4" s="325" t="s">
+      <c r="B4" s="332"/>
+      <c r="C4" s="332"/>
+      <c r="D4" s="332"/>
+      <c r="E4" s="332"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="329" t="s">
         <v>248</v>
       </c>
-      <c r="H4" s="325"/>
-      <c r="I4" s="325"/>
-      <c r="J4" s="325"/>
-      <c r="K4" s="325"/>
-      <c r="L4" s="325"/>
+      <c r="H4" s="329"/>
+      <c r="I4" s="329"/>
+      <c r="J4" s="329"/>
+      <c r="K4" s="329"/>
+      <c r="L4" s="329"/>
       <c r="M4" s="204" t="s">
         <v>252</v>
       </c>
@@ -9715,20 +9718,20 @@
       </c>
     </row>
     <row r="5" spans="1:17" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="330"/>
-      <c r="B5" s="331"/>
-      <c r="C5" s="331"/>
-      <c r="D5" s="331"/>
-      <c r="E5" s="331"/>
-      <c r="F5" s="332"/>
-      <c r="G5" s="334" t="s">
+      <c r="A5" s="324"/>
+      <c r="B5" s="325"/>
+      <c r="C5" s="325"/>
+      <c r="D5" s="325"/>
+      <c r="E5" s="325"/>
+      <c r="F5" s="326"/>
+      <c r="G5" s="345" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="334"/>
-      <c r="I5" s="334"/>
-      <c r="J5" s="334"/>
-      <c r="K5" s="334"/>
-      <c r="L5" s="334"/>
+      <c r="H5" s="345"/>
+      <c r="I5" s="345"/>
+      <c r="J5" s="345"/>
+      <c r="K5" s="345"/>
+      <c r="L5" s="345"/>
       <c r="M5" s="202" t="s">
         <v>291</v>
       </c>
@@ -9743,54 +9746,54 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="330"/>
-      <c r="B6" s="331"/>
-      <c r="C6" s="331"/>
-      <c r="D6" s="331"/>
-      <c r="E6" s="331"/>
-      <c r="F6" s="332"/>
-      <c r="G6" s="333"/>
-      <c r="H6" s="333"/>
-      <c r="I6" s="333"/>
-      <c r="J6" s="333"/>
-      <c r="K6" s="333"/>
-      <c r="L6" s="333"/>
+      <c r="A6" s="324"/>
+      <c r="B6" s="325"/>
+      <c r="C6" s="325"/>
+      <c r="D6" s="325"/>
+      <c r="E6" s="325"/>
+      <c r="F6" s="326"/>
+      <c r="G6" s="344"/>
+      <c r="H6" s="344"/>
+      <c r="I6" s="344"/>
+      <c r="J6" s="344"/>
+      <c r="K6" s="344"/>
+      <c r="L6" s="344"/>
       <c r="M6" s="205"/>
       <c r="N6" s="205"/>
       <c r="O6" s="205"/>
       <c r="P6" s="205"/>
     </row>
     <row r="7" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="330"/>
-      <c r="B7" s="331"/>
-      <c r="C7" s="331"/>
-      <c r="D7" s="331"/>
-      <c r="E7" s="331"/>
-      <c r="F7" s="332"/>
-      <c r="G7" s="333"/>
-      <c r="H7" s="333"/>
-      <c r="I7" s="333"/>
-      <c r="J7" s="333"/>
-      <c r="K7" s="333"/>
-      <c r="L7" s="333"/>
+      <c r="A7" s="324"/>
+      <c r="B7" s="325"/>
+      <c r="C7" s="325"/>
+      <c r="D7" s="325"/>
+      <c r="E7" s="325"/>
+      <c r="F7" s="326"/>
+      <c r="G7" s="344"/>
+      <c r="H7" s="344"/>
+      <c r="I7" s="344"/>
+      <c r="J7" s="344"/>
+      <c r="K7" s="344"/>
+      <c r="L7" s="344"/>
       <c r="M7" s="205"/>
       <c r="N7" s="205"/>
       <c r="O7" s="205"/>
       <c r="P7" s="206"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="330"/>
-      <c r="B8" s="331"/>
-      <c r="C8" s="331"/>
-      <c r="D8" s="331"/>
-      <c r="E8" s="331"/>
-      <c r="F8" s="332"/>
-      <c r="G8" s="333"/>
-      <c r="H8" s="333"/>
-      <c r="I8" s="333"/>
-      <c r="J8" s="333"/>
-      <c r="K8" s="333"/>
-      <c r="L8" s="333"/>
+      <c r="A8" s="324"/>
+      <c r="B8" s="325"/>
+      <c r="C8" s="325"/>
+      <c r="D8" s="325"/>
+      <c r="E8" s="325"/>
+      <c r="F8" s="326"/>
+      <c r="G8" s="344"/>
+      <c r="H8" s="344"/>
+      <c r="I8" s="344"/>
+      <c r="J8" s="344"/>
+      <c r="K8" s="344"/>
+      <c r="L8" s="344"/>
       <c r="M8" s="205"/>
       <c r="N8" s="205"/>
       <c r="O8" s="205"/>
@@ -9798,17 +9801,17 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:17" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="314" t="s">
+      <c r="A10" s="335" t="s">
         <v>353</v>
       </c>
-      <c r="B10" s="315"/>
-      <c r="C10" s="315"/>
-      <c r="D10" s="315"/>
-      <c r="E10" s="315"/>
-      <c r="F10" s="315"/>
-      <c r="G10" s="315"/>
-      <c r="H10" s="315"/>
-      <c r="I10" s="316"/>
+      <c r="B10" s="336"/>
+      <c r="C10" s="336"/>
+      <c r="D10" s="336"/>
+      <c r="E10" s="336"/>
+      <c r="F10" s="336"/>
+      <c r="G10" s="336"/>
+      <c r="H10" s="336"/>
+      <c r="I10" s="337"/>
     </row>
     <row r="11" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="129" t="s">
@@ -9823,7 +9826,7 @@
       <c r="D11" s="123" t="s">
         <v>270</v>
       </c>
-      <c r="E11" s="351" t="s">
+      <c r="E11" s="239" t="s">
         <v>270</v>
       </c>
       <c r="F11" s="123" t="s">
@@ -9853,7 +9856,7 @@
       <c r="D12" s="145" t="s">
         <v>94</v>
       </c>
-      <c r="E12" s="352" t="s">
+      <c r="E12" s="240" t="s">
         <v>513</v>
       </c>
       <c r="F12" s="145" t="s">
@@ -9897,69 +9900,69 @@
     </row>
     <row r="14" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="300" t="s">
+      <c r="A15" s="309" t="s">
         <v>280</v>
       </c>
-      <c r="B15" s="301"/>
-      <c r="C15" s="301"/>
-      <c r="D15" s="301"/>
-      <c r="E15" s="301"/>
-      <c r="F15" s="301"/>
-      <c r="G15" s="301"/>
-      <c r="H15" s="302"/>
+      <c r="B15" s="310"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="310"/>
+      <c r="E15" s="310"/>
+      <c r="F15" s="310"/>
+      <c r="G15" s="310"/>
+      <c r="H15" s="311"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="294" t="s">
+      <c r="A16" s="303" t="s">
         <v>363</v>
       </c>
-      <c r="B16" s="295"/>
-      <c r="C16" s="295"/>
-      <c r="D16" s="295"/>
-      <c r="E16" s="295"/>
-      <c r="F16" s="295"/>
-      <c r="G16" s="295"/>
-      <c r="H16" s="296"/>
+      <c r="B16" s="304"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="304"/>
+      <c r="E16" s="304"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="304"/>
+      <c r="H16" s="305"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="294"/>
-      <c r="B17" s="295"/>
-      <c r="C17" s="295"/>
-      <c r="D17" s="295"/>
-      <c r="E17" s="295"/>
-      <c r="F17" s="295"/>
-      <c r="G17" s="295"/>
-      <c r="H17" s="296"/>
+      <c r="A17" s="303"/>
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="304"/>
+      <c r="E17" s="304"/>
+      <c r="F17" s="304"/>
+      <c r="G17" s="304"/>
+      <c r="H17" s="305"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="294"/>
-      <c r="B18" s="295"/>
-      <c r="C18" s="295"/>
-      <c r="D18" s="295"/>
-      <c r="E18" s="295"/>
-      <c r="F18" s="295"/>
-      <c r="G18" s="295"/>
-      <c r="H18" s="296"/>
+      <c r="A18" s="303"/>
+      <c r="B18" s="304"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="304"/>
+      <c r="E18" s="304"/>
+      <c r="F18" s="304"/>
+      <c r="G18" s="304"/>
+      <c r="H18" s="305"/>
     </row>
     <row r="19" spans="1:8" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="297"/>
-      <c r="B19" s="298"/>
-      <c r="C19" s="298"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="298"/>
-      <c r="G19" s="298"/>
-      <c r="H19" s="299"/>
+      <c r="A19" s="306"/>
+      <c r="B19" s="307"/>
+      <c r="C19" s="307"/>
+      <c r="D19" s="307"/>
+      <c r="E19" s="307"/>
+      <c r="F19" s="307"/>
+      <c r="G19" s="307"/>
+      <c r="H19" s="308"/>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="284" t="s">
+      <c r="A21" s="293" t="s">
         <v>307</v>
       </c>
-      <c r="B21" s="284"/>
-      <c r="C21" s="284"/>
-      <c r="D21" s="284"/>
-      <c r="E21" s="284"/>
-      <c r="F21" s="284"/>
-      <c r="G21" s="284"/>
+      <c r="B21" s="293"/>
+      <c r="C21" s="293"/>
+      <c r="D21" s="293"/>
+      <c r="E21" s="293"/>
+      <c r="F21" s="293"/>
+      <c r="G21" s="293"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
@@ -9971,12 +9974,12 @@
       <c r="C22" s="77" t="s">
         <v>309</v>
       </c>
-      <c r="D22" s="283" t="s">
+      <c r="D22" s="292" t="s">
         <v>310</v>
       </c>
-      <c r="E22" s="283"/>
-      <c r="F22" s="283"/>
-      <c r="G22" s="283"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -10148,6 +10151,12 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="G3:L3"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="G2:L2"/>
+    <mergeCell ref="M2:P2"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A10:I10"/>
     <mergeCell ref="A21:G21"/>
@@ -10163,12 +10172,6 @@
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="G3:L3"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="G2:L2"/>
-    <mergeCell ref="M2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10234,8 +10237,8 @@
   </sheetPr>
   <dimension ref="A1:M85"/>
   <sheetViews>
-    <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10250,12 +10253,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="335" t="s">
+      <c r="A1" s="346" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="336"/>
-      <c r="C1" s="336"/>
-      <c r="D1" s="337"/>
+      <c r="B1" s="347"/>
+      <c r="C1" s="347"/>
+      <c r="D1" s="348"/>
       <c r="E1" s="65"/>
       <c r="F1" s="65"/>
       <c r="G1" s="65"/>
@@ -10330,7 +10333,7 @@
       <c r="B6" s="16" t="s">
         <v>515</v>
       </c>
-      <c r="C6" s="355"/>
+      <c r="C6" s="241"/>
       <c r="D6" s="23">
         <v>1000000</v>
       </c>
@@ -10342,7 +10345,9 @@
       <c r="B7" s="16" t="s">
         <v>516</v>
       </c>
-      <c r="C7" s="356"/>
+      <c r="C7" s="242" t="s">
+        <v>552</v>
+      </c>
       <c r="D7" s="23">
         <v>0</v>
       </c>
@@ -10354,7 +10359,7 @@
       <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="357"/>
+      <c r="C8" s="243"/>
       <c r="D8" s="23">
         <v>0</v>
       </c>
@@ -10366,7 +10371,7 @@
       <c r="B9" s="15" t="s">
         <v>518</v>
       </c>
-      <c r="C9" s="357"/>
+      <c r="C9" s="243"/>
       <c r="D9" s="23">
         <v>0</v>
       </c>
@@ -10378,7 +10383,7 @@
       <c r="B10" s="16" t="s">
         <v>520</v>
       </c>
-      <c r="C10" s="355"/>
+      <c r="C10" s="241"/>
       <c r="D10" s="23"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -10388,7 +10393,9 @@
       <c r="B11" s="16" t="s">
         <v>489</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="201">
+        <v>0</v>
+      </c>
       <c r="D11" s="23">
         <v>1</v>
       </c>
@@ -10400,7 +10407,7 @@
       <c r="B12" s="16" t="s">
         <v>522</v>
       </c>
-      <c r="C12" s="355"/>
+      <c r="C12" s="241"/>
       <c r="D12" s="23">
         <v>10000</v>
       </c>
@@ -10412,7 +10419,7 @@
       <c r="B13" s="16" t="s">
         <v>524</v>
       </c>
-      <c r="C13" s="355"/>
+      <c r="C13" s="241"/>
       <c r="D13" s="23">
         <v>0.1</v>
       </c>
@@ -10424,7 +10431,7 @@
       <c r="B14" s="16" t="s">
         <v>526</v>
       </c>
-      <c r="C14" s="355"/>
+      <c r="C14" s="241"/>
       <c r="D14" s="23"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -10434,7 +10441,7 @@
       <c r="B15" s="16" t="s">
         <v>528</v>
       </c>
-      <c r="C15" s="355"/>
+      <c r="C15" s="241"/>
       <c r="D15" s="23"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -10444,7 +10451,7 @@
       <c r="B16" s="16" t="s">
         <v>530</v>
       </c>
-      <c r="C16" s="355"/>
+      <c r="C16" s="241"/>
       <c r="D16" s="23">
         <v>10</v>
       </c>
@@ -10456,7 +10463,7 @@
       <c r="B17" s="16" t="s">
         <v>532</v>
       </c>
-      <c r="C17" s="355"/>
+      <c r="C17" s="241"/>
       <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -10466,7 +10473,7 @@
       <c r="B18" s="16" t="s">
         <v>534</v>
       </c>
-      <c r="C18" s="355"/>
+      <c r="C18" s="241"/>
       <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -10476,7 +10483,9 @@
       <c r="B19" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="C19" s="201"/>
+      <c r="C19" s="201">
+        <v>0</v>
+      </c>
       <c r="D19" s="23">
         <v>1</v>
       </c>
@@ -10834,8 +10843,8 @@
       <c r="B52" s="17" t="s">
         <v>536</v>
       </c>
-      <c r="C52" s="358"/>
-      <c r="D52" s="359"/>
+      <c r="C52" s="244"/>
+      <c r="D52" s="245"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
@@ -10844,8 +10853,8 @@
       <c r="B53" s="16" t="s">
         <v>538</v>
       </c>
-      <c r="C53" s="356"/>
-      <c r="D53" s="360">
+      <c r="C53" s="242"/>
+      <c r="D53" s="246">
         <v>0.02</v>
       </c>
     </row>
@@ -10856,8 +10865,8 @@
       <c r="B54" s="16" t="s">
         <v>540</v>
       </c>
-      <c r="C54" s="356"/>
-      <c r="D54" s="360"/>
+      <c r="C54" s="242"/>
+      <c r="D54" s="246"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
@@ -10866,8 +10875,8 @@
       <c r="B55" s="16" t="s">
         <v>542</v>
       </c>
-      <c r="C55" s="356"/>
-      <c r="D55" s="360"/>
+      <c r="C55" s="242"/>
+      <c r="D55" s="246"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
@@ -10876,8 +10885,8 @@
       <c r="B56" s="16" t="s">
         <v>544</v>
       </c>
-      <c r="C56" s="356"/>
-      <c r="D56" s="360"/>
+      <c r="C56" s="242"/>
+      <c r="D56" s="246"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
@@ -10886,7 +10895,7 @@
       <c r="B57" s="16" t="s">
         <v>546</v>
       </c>
-      <c r="C57" s="356"/>
+      <c r="C57" s="242"/>
       <c r="D57" s="24" t="s">
         <v>72</v>
       </c>
@@ -11149,7 +11158,7 @@
       <c r="A82" s="21" t="s">
         <v>548</v>
       </c>
-      <c r="B82" s="361" t="s">
+      <c r="B82" s="247" t="s">
         <v>549</v>
       </c>
       <c r="C82" s="179"/>
@@ -11204,7 +11213,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -11224,23 +11233,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="341" t="s">
+      <c r="A1" s="352" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="342"/>
-      <c r="C1" s="342"/>
-      <c r="D1" s="342"/>
-      <c r="E1" s="342"/>
-      <c r="F1" s="342"/>
-      <c r="G1" s="342"/>
-      <c r="H1" s="342"/>
-      <c r="I1" s="342"/>
-      <c r="J1" s="342"/>
-      <c r="K1" s="342"/>
-      <c r="L1" s="342"/>
-      <c r="M1" s="342"/>
-      <c r="N1" s="342"/>
-      <c r="O1" s="342"/>
+      <c r="B1" s="353"/>
+      <c r="C1" s="353"/>
+      <c r="D1" s="353"/>
+      <c r="E1" s="353"/>
+      <c r="F1" s="353"/>
+      <c r="G1" s="353"/>
+      <c r="H1" s="353"/>
+      <c r="I1" s="353"/>
+      <c r="J1" s="353"/>
+      <c r="K1" s="353"/>
+      <c r="L1" s="353"/>
+      <c r="M1" s="353"/>
+      <c r="N1" s="353"/>
+      <c r="O1" s="353"/>
     </row>
     <row r="2" spans="1:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -11258,17 +11267,17 @@
       <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:15" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="349" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="339"/>
-      <c r="I3" s="339"/>
-      <c r="J3" s="340"/>
+      <c r="C3" s="350"/>
+      <c r="D3" s="350"/>
+      <c r="E3" s="350"/>
+      <c r="F3" s="350"/>
+      <c r="G3" s="350"/>
+      <c r="H3" s="350"/>
+      <c r="I3" s="350"/>
+      <c r="J3" s="351"/>
     </row>
     <row r="4" spans="1:15" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B4" s="36"/>
@@ -11459,21 +11468,21 @@
     </row>
     <row r="18" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="2:14" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="338" t="s">
+      <c r="B19" s="349" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="339"/>
-      <c r="D19" s="339"/>
-      <c r="E19" s="339"/>
-      <c r="F19" s="339"/>
-      <c r="G19" s="339"/>
-      <c r="H19" s="339"/>
-      <c r="I19" s="339"/>
-      <c r="J19" s="339"/>
-      <c r="K19" s="339"/>
-      <c r="L19" s="339"/>
-      <c r="M19" s="339"/>
-      <c r="N19" s="340"/>
+      <c r="C19" s="350"/>
+      <c r="D19" s="350"/>
+      <c r="E19" s="350"/>
+      <c r="F19" s="350"/>
+      <c r="G19" s="350"/>
+      <c r="H19" s="350"/>
+      <c r="I19" s="350"/>
+      <c r="J19" s="350"/>
+      <c r="K19" s="350"/>
+      <c r="L19" s="350"/>
+      <c r="M19" s="350"/>
+      <c r="N19" s="351"/>
     </row>
     <row r="20" spans="2:14" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B20" s="36"/>
@@ -11675,27 +11684,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="346" t="s">
+      <c r="A1" s="357" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
-      <c r="H1" s="347"/>
-      <c r="I1" s="347"/>
-      <c r="J1" s="347"/>
-      <c r="K1" s="347"/>
-      <c r="L1" s="347"/>
-      <c r="M1" s="347"/>
-      <c r="N1" s="347"/>
-      <c r="O1" s="347"/>
-      <c r="P1" s="347"/>
-      <c r="Q1" s="347"/>
-      <c r="R1" s="347"/>
-      <c r="S1" s="347"/>
+      <c r="B1" s="358"/>
+      <c r="C1" s="358"/>
+      <c r="D1" s="358"/>
+      <c r="E1" s="358"/>
+      <c r="F1" s="358"/>
+      <c r="G1" s="358"/>
+      <c r="H1" s="358"/>
+      <c r="I1" s="358"/>
+      <c r="J1" s="358"/>
+      <c r="K1" s="358"/>
+      <c r="L1" s="358"/>
+      <c r="M1" s="358"/>
+      <c r="N1" s="358"/>
+      <c r="O1" s="358"/>
+      <c r="P1" s="358"/>
+      <c r="Q1" s="358"/>
+      <c r="R1" s="358"/>
+      <c r="S1" s="358"/>
     </row>
     <row r="2" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="34"/>
@@ -11709,26 +11718,26 @@
       <c r="I2" s="34"/>
     </row>
     <row r="3" spans="1:20" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="349" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="339"/>
-      <c r="I3" s="339"/>
-      <c r="J3" s="340"/>
-      <c r="L3" s="343" t="s">
+      <c r="C3" s="350"/>
+      <c r="D3" s="350"/>
+      <c r="E3" s="350"/>
+      <c r="F3" s="350"/>
+      <c r="G3" s="350"/>
+      <c r="H3" s="350"/>
+      <c r="I3" s="350"/>
+      <c r="J3" s="351"/>
+      <c r="L3" s="354" t="s">
         <v>223</v>
       </c>
-      <c r="M3" s="344"/>
-      <c r="N3" s="344"/>
-      <c r="O3" s="344"/>
-      <c r="P3" s="344"/>
-      <c r="Q3" s="344"/>
-      <c r="R3" s="345"/>
+      <c r="M3" s="355"/>
+      <c r="N3" s="355"/>
+      <c r="O3" s="355"/>
+      <c r="P3" s="355"/>
+      <c r="Q3" s="355"/>
+      <c r="R3" s="356"/>
       <c r="S3" s="35"/>
       <c r="T3" s="35"/>
     </row>
@@ -11959,23 +11968,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="348" t="s">
+      <c r="A1" s="359" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="349"/>
-      <c r="C1" s="349"/>
-      <c r="D1" s="349"/>
-      <c r="E1" s="349"/>
-      <c r="F1" s="349"/>
-      <c r="G1" s="349"/>
-      <c r="H1" s="349"/>
-      <c r="I1" s="349"/>
-      <c r="J1" s="349"/>
-      <c r="K1" s="349"/>
-      <c r="L1" s="349"/>
-      <c r="M1" s="349"/>
-      <c r="N1" s="349"/>
-      <c r="O1" s="350"/>
+      <c r="B1" s="360"/>
+      <c r="C1" s="360"/>
+      <c r="D1" s="360"/>
+      <c r="E1" s="360"/>
+      <c r="F1" s="360"/>
+      <c r="G1" s="360"/>
+      <c r="H1" s="360"/>
+      <c r="I1" s="360"/>
+      <c r="J1" s="360"/>
+      <c r="K1" s="360"/>
+      <c r="L1" s="360"/>
+      <c r="M1" s="360"/>
+      <c r="N1" s="360"/>
+      <c r="O1" s="361"/>
     </row>
     <row r="2" spans="1:16" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33"/>
@@ -11988,22 +11997,22 @@
       <c r="H2" s="51"/>
     </row>
     <row r="3" spans="1:16" ht="29.25" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B3" s="338" t="s">
+      <c r="B3" s="349" t="s">
         <v>223</v>
       </c>
-      <c r="C3" s="339"/>
-      <c r="D3" s="339"/>
-      <c r="E3" s="339"/>
-      <c r="F3" s="339"/>
-      <c r="G3" s="339"/>
-      <c r="H3" s="340"/>
-      <c r="J3" s="343" t="s">
+      <c r="C3" s="350"/>
+      <c r="D3" s="350"/>
+      <c r="E3" s="350"/>
+      <c r="F3" s="350"/>
+      <c r="G3" s="350"/>
+      <c r="H3" s="351"/>
+      <c r="J3" s="354" t="s">
         <v>223</v>
       </c>
-      <c r="K3" s="344"/>
-      <c r="L3" s="344"/>
-      <c r="M3" s="344"/>
-      <c r="N3" s="345"/>
+      <c r="K3" s="355"/>
+      <c r="L3" s="355"/>
+      <c r="M3" s="355"/>
+      <c r="N3" s="356"/>
       <c r="O3" s="35"/>
       <c r="P3" s="35"/>
     </row>

</xml_diff>